<commit_message>
Removed Batch Run job related test cases in DecoratorTestData excel
</commit_message>
<xml_diff>
--- a/src/test/test-data/DecoratorTestData.xlsx
+++ b/src/test/test-data/DecoratorTestData.xlsx
@@ -8,16 +8,17 @@
   </bookViews>
   <sheets>
     <sheet name="Decorator" sheetId="2" r:id="rId1"/>
+    <sheet name="Back_UP" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Decorator!$A$1:$L$50</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Decorator!$A$1:$L$44</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="208">
   <si>
     <t>API</t>
   </si>
@@ -685,6 +686,9 @@
   </si>
   <si>
     <t>/follow/user/(OPQA-2706_userid)/following/(OPQA-2706_3_userid)</t>
+  </si>
+  <si>
+    <t>Verify that user create comment in  article</t>
   </si>
 </sst>
 </file>
@@ -766,7 +770,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -800,6 +804,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1095,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L50"/>
+  <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L50"/>
+    <sheetView tabSelected="1" topLeftCell="H39" workbookViewId="0">
+      <selection activeCell="L44" sqref="L2:L44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1637,6 +1644,1354 @@
       <c r="I18" s="5" t="s">
         <v>92</v>
       </c>
+      <c r="J18" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="K18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="60">
+      <c r="A19" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" ht="60">
+      <c r="A20" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" ht="60">
+      <c r="A21" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
+        <v>179</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="K21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="150">
+      <c r="A22" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I22" s="8"/>
+      <c r="J22" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30">
+      <c r="A23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" t="s">
+        <v>176</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="K23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30">
+      <c r="A24" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" t="s">
+        <v>194</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="K24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30">
+      <c r="A25" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G25" s="8"/>
+      <c r="H25" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="K25" s="8"/>
+    </row>
+    <row r="26" spans="1:11" ht="30">
+      <c r="A26" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="G26" s="8"/>
+      <c r="H26" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="K26" s="8"/>
+    </row>
+    <row r="27" spans="1:11" ht="90">
+      <c r="A27" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" t="s">
+        <v>179</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I27" t="s">
+        <v>57</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="K27" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="45">
+      <c r="A28" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="I28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="30">
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="30">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" t="s">
+        <v>26</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="90">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" t="s">
+        <v>179</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I31" t="s">
+        <v>68</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="K31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="75">
+      <c r="A32" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" t="s">
+        <v>196</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I32" t="s">
+        <v>97</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="45">
+      <c r="A33" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="G33" s="8"/>
+      <c r="H33" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="I33" t="s">
+        <v>43</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="K33" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="60">
+      <c r="A34" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" t="s">
+        <v>194</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="K34" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="60">
+      <c r="A35" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" t="s">
+        <v>176</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="K35" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="45">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" t="s">
+        <v>179</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I36" t="s">
+        <v>72</v>
+      </c>
+      <c r="J36" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="K36" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="30">
+      <c r="A37" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G37" s="8"/>
+      <c r="H37" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K37" s="8"/>
+    </row>
+    <row r="38" spans="1:11" ht="30">
+      <c r="A38" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J38" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="90">
+      <c r="A39" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" t="s">
+        <v>204</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I39" t="s">
+        <v>86</v>
+      </c>
+      <c r="J39" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="K39" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="45">
+      <c r="A40" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C40" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G40" s="8"/>
+      <c r="H40" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I40" t="s">
+        <v>116</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="30">
+      <c r="A41" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" t="s">
+        <v>176</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="K41" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="30">
+      <c r="A42" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" t="s">
+        <v>176</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="K42" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11">
+      <c r="A43" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H43"/>
+      <c r="J43" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11">
+      <c r="A44" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H44"/>
+      <c r="J44" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:L44">
+    <filterColumn colId="2"/>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:L50"/>
+  <sheetViews>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="73" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="87.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="47.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="52.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="61.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="65.7109375" style="5" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="105">
+      <c r="A2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30">
+      <c r="A3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="I3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="105">
+      <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30">
+      <c r="A5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="I5" t="s">
+        <v>164</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="105">
+      <c r="A6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30">
+      <c r="A7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>155</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="I7" t="s">
+        <v>166</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="105">
+      <c r="A8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30">
+      <c r="A9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="I9" t="s">
+        <v>167</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30">
+      <c r="A11" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="H11"/>
+      <c r="J11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" ht="30">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>179</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I13" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="K13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="4"/>
+      <c r="J14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" ht="30">
+      <c r="A15" t="s">
+        <v>205</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" ht="60">
+      <c r="A16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>176</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="K16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="120">
+      <c r="A17" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="60">
+      <c r="A18" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" t="s">
+        <v>179</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="J18" s="5" t="s">
         <v>192</v>
       </c>

</xml_diff>

<commit_message>
Committing Ramesh latest file
</commit_message>
<xml_diff>
--- a/src/test/test-data/DecoratorTestData.xlsx
+++ b/src/test/test-data/DecoratorTestData.xlsx
@@ -4,21 +4,24 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2580" windowWidth="19440" windowHeight="5385"/>
+    <workbookView xWindow="0" yWindow="2580" windowWidth="15600" windowHeight="5385"/>
   </bookViews>
   <sheets>
     <sheet name="Decorator" sheetId="2" r:id="rId1"/>
     <sheet name="Back_UP" sheetId="3" r:id="rId2"/>
+    <sheet name="NewUsers" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Decorator!$A$1:$L$44</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Decorator!$A$1:$L$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NewUsers!$A$1:$L$44</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="852" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="234">
   <si>
     <t>API</t>
   </si>
@@ -689,6 +692,84 @@
   </si>
   <si>
     <t>Verify that user create comment in  article</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=FOLLOW||notify.issuerProfile.truid=(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER1)||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>/follow/user/(SYS_USER1)/following/(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER2)||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER2)||found=true</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=POST_CREATED||notify.post.id=(OPQA-360_id)||notify.post.issuerProfile.truid=(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=POST_CREATED||notify.post.id=(OPQA-360_id)||notify.issuerProfile.truid=(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER2)</t>
+  </si>
+  <si>
+    <t>/follow/user/(SYS_USER2)/following/(SYS_USER3)</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=FRIENDS_FOLLOWED_OTHERS||notify.issuerProfile.truid=(SYS_USER2)||notify.followingUsers.profile.truid=(SYS_USER3)</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER3)||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename==PUBLIC_WATCHLIST||notify.issuerProfile.truid=(SYS_USER3)||notify.publication.containerId=(OPQA-312_containerId)||notify.action=CREATE_WATCHLIST</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER3)</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=AppreciationEvent||notify.profilesByGroup.profile.truid=(SYS_USER3)||notify.profilesByGroup.profile.truid=(SYS_USER1)||notify.publicationRef.comment.id=(OPQA-236_comments.id)||notify.publicationRef.comment.content=Notification Test</t>
+  </si>
+  <si>
+    <t>x-1p-user=(SYS_USER3)</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=AppreciationEvent||notify.profilesByGroup.profile.truid=(SYS_USER3)||notify.profilesByGroup.profile.truid=(SYS_USER1)||notify.publicationRef.comment.id=(OPQA-385_comments.id)||notify.publicationRef.comment.content=Notification Test (ddMMMyyyy_HHmmss)</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER4)||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER4)||comments.targetType=Post||comments.targetId=(OPQA-360_id)||comments.content=Notification Test</t>
+  </si>
+  <si>
+    <t>X-1P-User=(SYS_USER4)</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=AppreciationEvent||notify.issuer=(SYS_USER3)||notify.issuer=(SYS_USER1)||notify.publicationRef.comment.post.id=(OPQA-360_id)||notify.publicationRef.comment.post.title=Creating Post For API Notification Testing</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=PUBLIC_WATCHLIST||notify.issuerProfile.truid=(SYS_USER3)||notify.publication.containerId=(OPQA-312_containerId)||notify.action=EDIT_PERMISSIONS_IN_WATCHLIST</t>
+  </si>
+  <si>
+    <t>status=200||notify.cause=MyDocumentComment||notify.issuer=(SYS_USER4)||notify.comments.content=Notification Test (ddMMMyyyy_HHmmss)||notify.id=(OPQA-360_id)</t>
+  </si>
+  <si>
+    <t>status=200||notify.cause=WatchedDocumentComment||notify.issuerProfile.truid=(SYS_USER4)||notify.comments.content=Notification Test (ddMMMyyyy_HHmmss)||notify.id=(OPQA-360_id)</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=DocumentCommentPost||notify.issuerProfile.truid=(SYS_USER4)||notify.comments.content=Notification Test (ddMMMyyyy_HHmmss)||notify.id=(OPQA-360_id)</t>
   </si>
 </sst>
 </file>
@@ -1102,10 +1183,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L44"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H39" workbookViewId="0">
-      <selection activeCell="L44" sqref="L2:L44"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="L2" sqref="L2:L41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1162,469 +1243,495 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:12" ht="105">
+    <row r="2" spans="1:12">
       <c r="A2" t="s">
-        <v>151</v>
+        <v>14</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>152</v>
+        <v>20</v>
       </c>
       <c r="C2" t="s">
-        <v>153</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="E2" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>163</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H2" s="4"/>
+      <c r="I2" s="1"/>
       <c r="J2" s="5" t="s">
         <v>12</v>
       </c>
+      <c r="K2" s="1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="30">
-      <c r="A3" t="s">
-        <v>162</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C3" t="s">
-        <v>158</v>
+      <c r="A3" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F3" t="s">
-        <v>155</v>
-      </c>
-      <c r="H3" s="5" t="s">
-        <v>160</v>
-      </c>
-      <c r="I3" t="s">
-        <v>151</v>
-      </c>
-      <c r="J3" s="5" t="s">
+        <v>118</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="H3"/>
+      <c r="J3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="K3" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="105">
+      <c r="K3" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
-        <v>164</v>
+        <v>33</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>152</v>
+        <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>153</v>
-      </c>
-      <c r="D4" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="E4" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>170</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>211</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="1"/>
       <c r="J4" s="5" t="s">
-        <v>12</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>37</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C5" t="s">
-        <v>158</v>
+        <v>38</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="E5" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F5" t="s">
-        <v>155</v>
+        <v>212</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="I5" t="s">
-        <v>164</v>
+        <v>33</v>
       </c>
       <c r="J5" s="5" t="s">
-        <v>12</v>
+        <v>208</v>
       </c>
       <c r="K5" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="105">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12">
       <c r="A6" t="s">
-        <v>166</v>
+        <v>39</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>152</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>153</v>
-      </c>
-      <c r="D6" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="E6" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>171</v>
-      </c>
+        <v>35</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="4"/>
       <c r="J6" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="30">
-      <c r="A7" t="s">
-        <v>156</v>
+        <v>36</v>
+      </c>
+      <c r="K6" s="1"/>
+    </row>
+    <row r="7" spans="1:12" ht="45">
+      <c r="A7" s="8" t="s">
+        <v>41</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C7" t="s">
-        <v>158</v>
+        <v>42</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="E7" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F7" t="s">
-        <v>155</v>
+        <v>209</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>172</v>
+        <v>136</v>
       </c>
       <c r="I7" t="s">
-        <v>166</v>
+        <v>39</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>12</v>
+        <v>219</v>
       </c>
       <c r="K7" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="105">
-      <c r="A8" t="s">
-        <v>167</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="120">
+      <c r="A8" s="5" t="s">
+        <v>92</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>152</v>
+        <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>153</v>
-      </c>
-      <c r="D8" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="E8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>155</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>173</v>
-      </c>
+        <v>220</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I8" s="1"/>
       <c r="J8" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="30">
-      <c r="A9" t="s">
-        <v>168</v>
+        <v>19</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45">
+      <c r="A9" s="5" t="s">
+        <v>107</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>157</v>
-      </c>
-      <c r="C9" t="s">
-        <v>158</v>
+        <v>106</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>159</v>
-      </c>
-      <c r="E9" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F9" t="s">
-        <v>155</v>
+        <v>212</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>174</v>
-      </c>
-      <c r="I9" t="s">
-        <v>167</v>
-      </c>
-      <c r="J9" s="5" t="s">
-        <v>12</v>
+        <v>136</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J9" s="15" t="s">
+        <v>221</v>
       </c>
       <c r="K9" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12">
-      <c r="A10" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>20</v>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="60">
+      <c r="A10" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>110</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>22</v>
+        <v>102</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H10" s="4"/>
-      <c r="I10" s="1"/>
+        <v>101</v>
+      </c>
+      <c r="F10" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="G10" s="5"/>
+      <c r="H10" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="I10" s="5" t="s">
+        <v>92</v>
+      </c>
       <c r="J10" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K10" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="30">
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:12" ht="60">
       <c r="A11" s="4" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>21</v>
+        <v>111</v>
+      </c>
+      <c r="C11" t="s">
+        <v>16</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="G11" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="H11"/>
-      <c r="J11" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="E11" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>220</v>
+      </c>
+      <c r="G11" s="5"/>
+      <c r="H11" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K11" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="30">
-      <c r="A12" t="s">
-        <v>33</v>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:12" ht="45">
+      <c r="A12" s="5" t="s">
+        <v>105</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C12" t="s">
-        <v>35</v>
+        <v>104</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>178</v>
+        <v>135</v>
       </c>
       <c r="E12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="4"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K12" s="1"/>
-    </row>
-    <row r="13" spans="1:12" ht="30">
-      <c r="A13" t="s">
-        <v>37</v>
+      <c r="F12" t="s">
+        <v>212</v>
+      </c>
+      <c r="H12" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I12" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="K12" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="150">
+      <c r="A13" s="8" t="s">
+        <v>43</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C13" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C13" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="G13" s="8"/>
+      <c r="H13" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30">
+      <c r="A14" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C14" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D14" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E13" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F13" t="s">
-        <v>179</v>
-      </c>
-      <c r="H13" s="5" t="s">
+      <c r="E14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
+        <v>209</v>
+      </c>
+      <c r="H14" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="I13" t="s">
-        <v>33</v>
-      </c>
-      <c r="J13" s="5" t="s">
-        <v>175</v>
-      </c>
-      <c r="K13" t="s">
+      <c r="I14" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J14" s="5" t="s">
+        <v>215</v>
+      </c>
+      <c r="K14" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:12">
-      <c r="A14" t="s">
-        <v>39</v>
-      </c>
-      <c r="B14" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="C14" t="s">
-        <v>35</v>
-      </c>
-      <c r="D14" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="4"/>
-      <c r="J14" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K14" s="1"/>
-    </row>
     <row r="15" spans="1:12" ht="30">
-      <c r="A15" t="s">
-        <v>205</v>
+      <c r="A15" s="8" t="s">
+        <v>114</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" t="s">
-        <v>35</v>
+        <v>115</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>206</v>
+        <v>135</v>
       </c>
       <c r="E15" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="1"/>
+      <c r="F15" t="s">
+        <v>222</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I15" s="8" t="s">
+        <v>43</v>
+      </c>
       <c r="J15" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" ht="60">
+        <v>216</v>
+      </c>
+      <c r="K15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" ht="30">
       <c r="A16" s="8" t="s">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>134</v>
+        <v>51</v>
+      </c>
+      <c r="C16" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E16" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F16" t="s">
-        <v>176</v>
-      </c>
-      <c r="H16" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="I16" t="s">
-        <v>39</v>
-      </c>
-      <c r="J16" s="5" t="s">
-        <v>190</v>
-      </c>
-      <c r="K16" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="17" spans="1:11" ht="120">
-      <c r="A17" s="5" t="s">
-        <v>92</v>
+        <v>52</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="G16" s="8"/>
+      <c r="H16" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I16" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J16" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="K16" s="8"/>
+    </row>
+    <row r="17" spans="1:11" ht="30">
+      <c r="A17" s="8" t="s">
+        <v>54</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C17" t="s">
-        <v>16</v>
+        <v>51</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="G17" s="5"/>
-      <c r="H17" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="I17" s="1"/>
-      <c r="J17" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="K17" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="60">
+        <v>52</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="G17" s="8"/>
+      <c r="H17" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I17" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J17" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="K17" s="8"/>
+    </row>
+    <row r="18" spans="1:11" ht="75">
       <c r="A18" s="5" t="s">
-        <v>107</v>
+        <v>55</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>106</v>
+        <v>56</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>134</v>
@@ -1636,278 +1743,276 @@
         <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>179</v>
+        <v>212</v>
       </c>
       <c r="H18" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="I18" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>192</v>
+      <c r="I18" t="s">
+        <v>57</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>229</v>
       </c>
       <c r="K18" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="60">
-      <c r="A19" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>110</v>
+    <row r="19" spans="1:11" ht="45">
+      <c r="A19" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>207</v>
       </c>
       <c r="C19" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F19" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="G19" s="8"/>
+      <c r="H19" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="I19" t="s">
+        <v>14</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" ht="30">
+      <c r="A20" t="s">
+        <v>60</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E20" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I20" t="s">
+        <v>26</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" ht="30">
+      <c r="A21" t="s">
+        <v>64</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C21" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E21" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" s="9" t="s">
+        <v>220</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="75">
+      <c r="A22" t="s">
+        <v>66</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" t="s">
+        <v>212</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I22" t="s">
+        <v>68</v>
+      </c>
+      <c r="J22" s="5" t="s">
+        <v>223</v>
+      </c>
+      <c r="K22" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="75">
+      <c r="A23" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C23" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="6" t="s">
-        <v>102</v>
-      </c>
-      <c r="E19" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="G19" s="5"/>
-      <c r="H19" s="4" t="s">
-        <v>139</v>
-      </c>
-      <c r="I19" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J19" s="5" t="s">
+      <c r="D23" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" t="s">
+        <v>224</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I23" t="s">
+        <v>97</v>
+      </c>
+      <c r="J23" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="K19" s="1"/>
-    </row>
-    <row r="20" spans="1:11" ht="60">
-      <c r="A20" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="C20" t="s">
-        <v>16</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>191</v>
-      </c>
-      <c r="G20" s="5"/>
-      <c r="H20" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J20" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K20" s="1"/>
-    </row>
-    <row r="21" spans="1:11" ht="60">
-      <c r="A21" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="B21" s="5" t="s">
-        <v>104</v>
-      </c>
-      <c r="C21" s="1" t="s">
+    </row>
+    <row r="24" spans="1:11" ht="45">
+      <c r="A24" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C24" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E24" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" s="9" t="s">
+        <v>226</v>
+      </c>
+      <c r="G24" s="8"/>
+      <c r="H24" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="I24" t="s">
+        <v>43</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="K24" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="45">
+      <c r="A25" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D25" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E21" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" t="s">
-        <v>179</v>
-      </c>
-      <c r="H21" s="5" t="s">
+      <c r="E25" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" t="s">
+        <v>222</v>
+      </c>
+      <c r="H25" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="I21" s="5" t="s">
-        <v>92</v>
-      </c>
-      <c r="J21" s="15" t="s">
-        <v>193</v>
-      </c>
-      <c r="K21" t="s">
+      <c r="I25" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>232</v>
+      </c>
+      <c r="K25" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="150">
-      <c r="A22" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="B22" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="C22" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F22" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="G22" s="8"/>
-      <c r="H22" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="I22" s="8"/>
-      <c r="J22" s="9" t="s">
-        <v>181</v>
-      </c>
-      <c r="K22" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" ht="30">
-      <c r="A23" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="B23" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="1" t="s">
+    <row r="26" spans="1:11" ht="45">
+      <c r="A26" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D26" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" t="s">
-        <v>176</v>
-      </c>
-      <c r="H23" s="5" t="s">
+      <c r="E26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" t="s">
+        <v>209</v>
+      </c>
+      <c r="H26" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="I23" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="K23" t="s">
+      <c r="I26" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="K26" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="30">
-      <c r="A24" s="8" t="s">
-        <v>114</v>
-      </c>
-      <c r="B24" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E24" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F24" t="s">
-        <v>194</v>
-      </c>
-      <c r="H24" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="I24" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="J24" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="K24" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="30">
-      <c r="A25" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B25" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C25" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E25" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F25" s="11" t="s">
-        <v>177</v>
-      </c>
-      <c r="G25" s="8"/>
-      <c r="H25" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="I25" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="J25" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="K25" s="8"/>
-    </row>
-    <row r="26" spans="1:11" ht="30">
-      <c r="A26" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="I26" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="K26" s="8"/>
-    </row>
-    <row r="27" spans="1:11" ht="90">
-      <c r="A27" s="5" t="s">
-        <v>55</v>
+    <row r="27" spans="1:11" ht="45">
+      <c r="A27" t="s">
+        <v>74</v>
       </c>
       <c r="B27" s="5" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>134</v>
@@ -1919,531 +2024,247 @@
         <v>13</v>
       </c>
       <c r="F27" t="s">
-        <v>179</v>
+        <v>212</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>136</v>
       </c>
       <c r="I27" t="s">
-        <v>57</v>
-      </c>
-      <c r="J27" s="5" t="s">
-        <v>195</v>
+        <v>72</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>231</v>
       </c>
       <c r="K27" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="45">
+    <row r="28" spans="1:11" ht="30">
       <c r="A28" s="8" t="s">
-        <v>26</v>
+        <v>80</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E28" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="E28" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F28" s="9" t="s">
-        <v>180</v>
+        <v>210</v>
       </c>
       <c r="G28" s="8"/>
-      <c r="H28" s="4" t="s">
-        <v>142</v>
-      </c>
-      <c r="I28" t="s">
-        <v>14</v>
-      </c>
-      <c r="J28" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="K28" s="8" t="s">
-        <v>29</v>
-      </c>
+      <c r="H28" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K28" s="8"/>
     </row>
     <row r="29" spans="1:11" ht="30">
-      <c r="A29" t="s">
-        <v>60</v>
+      <c r="A29" s="8" t="s">
+        <v>84</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C29" t="s">
+        <v>83</v>
+      </c>
+      <c r="C29" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
       <c r="E29" t="s">
         <v>13</v>
       </c>
       <c r="F29" s="9" t="s">
-        <v>177</v>
+        <v>220</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="I29" t="s">
-        <v>26</v>
-      </c>
-      <c r="J29" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="30">
+      <c r="I29" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J29" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="75">
       <c r="A30" t="s">
-        <v>64</v>
+        <v>112</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C30" t="s">
+        <v>113</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E30" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" t="s">
+        <v>228</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I30" t="s">
+        <v>86</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>225</v>
+      </c>
+      <c r="K30" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="45">
+      <c r="A31" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C31" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E30" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I30" t="s">
-        <v>26</v>
-      </c>
-      <c r="J30" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="90">
-      <c r="A31" t="s">
-        <v>66</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="C31" s="1" t="s">
+      <c r="D31" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="G31" s="8"/>
+      <c r="H31" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I31" t="s">
+        <v>116</v>
+      </c>
+      <c r="J31" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="30">
+      <c r="A32" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C32" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" t="s">
-        <v>179</v>
-      </c>
-      <c r="H31" s="5" t="s">
+      <c r="E32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" t="s">
+        <v>209</v>
+      </c>
+      <c r="H32" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="I31" t="s">
-        <v>68</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>197</v>
-      </c>
-      <c r="K31" t="s">
+      <c r="J32" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="K32" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="75">
-      <c r="A32" s="5" t="s">
-        <v>100</v>
-      </c>
-      <c r="B32" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C32" t="s">
-        <v>16</v>
-      </c>
-      <c r="D32" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" t="s">
-        <v>196</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I32" t="s">
-        <v>97</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="45">
-      <c r="A33" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="B33" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>27</v>
+    <row r="33" spans="1:11" ht="30">
+      <c r="A33" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="D33" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" s="9" t="s">
-        <v>199</v>
-      </c>
-      <c r="G33" s="8"/>
-      <c r="H33" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="I33" t="s">
-        <v>43</v>
-      </c>
-      <c r="J33" s="9" t="s">
-        <v>200</v>
-      </c>
-      <c r="K33" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11" ht="60">
-      <c r="A34" s="8" t="s">
-        <v>76</v>
+        <v>135</v>
+      </c>
+      <c r="E33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" t="s">
+        <v>209</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="K33" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="s">
+        <v>87</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>134</v>
+        <v>88</v>
+      </c>
+      <c r="C34" t="s">
+        <v>35</v>
       </c>
       <c r="D34" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E34" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F34" t="s">
-        <v>194</v>
-      </c>
-      <c r="H34" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="I34" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="J34" s="9" t="s">
-        <v>201</v>
-      </c>
-      <c r="K34" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11" ht="60">
-      <c r="A35" s="8" t="s">
-        <v>78</v>
+        <v>211</v>
+      </c>
+      <c r="E34" t="s">
+        <v>32</v>
+      </c>
+      <c r="H34"/>
+      <c r="J34" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" t="s">
+        <v>90</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>134</v>
+        <v>88</v>
+      </c>
+      <c r="C35" t="s">
+        <v>35</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E35" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F35" t="s">
-        <v>176</v>
-      </c>
-      <c r="H35" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="I35" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="J35" s="9" t="s">
-        <v>202</v>
-      </c>
-      <c r="K35" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="45">
-      <c r="A36" t="s">
-        <v>74</v>
-      </c>
-      <c r="B36" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C36" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D36" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E36" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F36" t="s">
-        <v>179</v>
-      </c>
-      <c r="H36" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="I36" t="s">
-        <v>72</v>
-      </c>
-      <c r="J36" s="9" t="s">
-        <v>203</v>
-      </c>
-      <c r="K36" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="30">
-      <c r="A37" s="8" t="s">
-        <v>80</v>
-      </c>
-      <c r="B37" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D37" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F37" s="9" t="s">
-        <v>177</v>
-      </c>
-      <c r="G37" s="8"/>
-      <c r="H37" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="I37" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="J37" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="K37" s="8"/>
-    </row>
-    <row r="38" spans="1:11" ht="30">
-      <c r="A38" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B38" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D38" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E38" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>191</v>
-      </c>
-      <c r="H38" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I38" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="J38" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="39" spans="1:11" ht="90">
-      <c r="A39" t="s">
-        <v>112</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D39" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" t="s">
-        <v>204</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="I39" t="s">
-        <v>86</v>
-      </c>
-      <c r="J39" s="9" t="s">
-        <v>198</v>
-      </c>
-      <c r="K39" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="40" spans="1:11" ht="45">
-      <c r="A40" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B40" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C40" t="s">
-        <v>27</v>
-      </c>
-      <c r="D40" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E40" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F40" s="9" t="s">
-        <v>180</v>
-      </c>
-      <c r="G40" s="8"/>
-      <c r="H40" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="I40" t="s">
-        <v>116</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>184</v>
-      </c>
-      <c r="K40" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" ht="30">
-      <c r="A41" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="B41" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D41" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F41" t="s">
-        <v>176</v>
-      </c>
-      <c r="H41" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="J41" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="K41" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="42" spans="1:11" ht="30">
-      <c r="A42" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D42" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E42" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F42" t="s">
-        <v>176</v>
-      </c>
-      <c r="H42" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="J42" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="K42" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="43" spans="1:11">
-      <c r="A43" t="s">
-        <v>87</v>
-      </c>
-      <c r="B43" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C43" t="s">
-        <v>35</v>
-      </c>
-      <c r="D43" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="E43" t="s">
+        <v>218</v>
+      </c>
+      <c r="E35" t="s">
         <v>32</v>
       </c>
-      <c r="H43"/>
-      <c r="J43" s="5" t="s">
+      <c r="H35"/>
+      <c r="J35" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:11">
-      <c r="A44" t="s">
-        <v>90</v>
-      </c>
-      <c r="B44" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C44" t="s">
-        <v>35</v>
-      </c>
-      <c r="D44" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="E44" t="s">
-        <v>32</v>
-      </c>
-      <c r="H44"/>
-      <c r="J44" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:L44">
-    <filterColumn colId="2"/>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -2452,8 +2273,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L63"/>
+    <sheetView topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3977,4 +3798,1371 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:L44"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="73" style="5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="16" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="87.85546875" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="47.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="52.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="61.85546875" style="5" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="65.7109375" style="5" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="105" hidden="1">
+      <c r="A2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="30" hidden="1">
+      <c r="A3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C3" t="s">
+        <v>158</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" t="s">
+        <v>155</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="I3" t="s">
+        <v>151</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="105" hidden="1">
+      <c r="A4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C4" t="s">
+        <v>153</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>170</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="30" hidden="1">
+      <c r="A5" t="s">
+        <v>165</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C5" t="s">
+        <v>158</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>169</v>
+      </c>
+      <c r="I5" t="s">
+        <v>164</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K5" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="105" hidden="1">
+      <c r="A6" t="s">
+        <v>166</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" t="s">
+        <v>153</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="E6" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="J6" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="30" hidden="1">
+      <c r="A7" t="s">
+        <v>156</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C7" t="s">
+        <v>158</v>
+      </c>
+      <c r="D7" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F7" t="s">
+        <v>155</v>
+      </c>
+      <c r="H7" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="I7" t="s">
+        <v>166</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K7" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="105" hidden="1">
+      <c r="A8" t="s">
+        <v>167</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" t="s">
+        <v>153</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>154</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="5" t="s">
+        <v>155</v>
+      </c>
+      <c r="H8" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="30" hidden="1">
+      <c r="A9" t="s">
+        <v>168</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>157</v>
+      </c>
+      <c r="C9" t="s">
+        <v>158</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>159</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" t="s">
+        <v>155</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="I9" t="s">
+        <v>167</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" hidden="1">
+      <c r="A10" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F10" s="1"/>
+      <c r="G10" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="H10" s="4"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="30" hidden="1">
+      <c r="A11" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="H11"/>
+      <c r="J11" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="30" hidden="1">
+      <c r="A12" t="s">
+        <v>33</v>
+      </c>
+      <c r="B12" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="1"/>
+      <c r="J12" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:12" ht="30">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F13" t="s">
+        <v>179</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I13" t="s">
+        <v>33</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="K13" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" hidden="1">
+      <c r="A14" t="s">
+        <v>39</v>
+      </c>
+      <c r="B14" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C14" t="s">
+        <v>35</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="4"/>
+      <c r="J14" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K14" s="1"/>
+    </row>
+    <row r="15" spans="1:12" ht="30" hidden="1">
+      <c r="A15" t="s">
+        <v>205</v>
+      </c>
+      <c r="B15" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" ht="60">
+      <c r="A16" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F16" t="s">
+        <v>176</v>
+      </c>
+      <c r="H16" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I16" t="s">
+        <v>39</v>
+      </c>
+      <c r="J16" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="K16" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" ht="120" hidden="1">
+      <c r="A17" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B17" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="G17" s="5"/>
+      <c r="H17" s="4" t="s">
+        <v>138</v>
+      </c>
+      <c r="I17" s="1"/>
+      <c r="J17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" ht="60">
+      <c r="A18" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F18" t="s">
+        <v>179</v>
+      </c>
+      <c r="H18" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I18" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J18" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="K18" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" ht="60" hidden="1">
+      <c r="A19" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>102</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="G19" s="5"/>
+      <c r="H19" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K19" s="1"/>
+    </row>
+    <row r="20" spans="1:11" ht="60" hidden="1">
+      <c r="A20" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="C20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="E20" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="F20" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="G20" s="5"/>
+      <c r="H20" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="I20" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K20" s="1"/>
+    </row>
+    <row r="21" spans="1:11" ht="60">
+      <c r="A21" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
+        <v>179</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="J21" s="15" t="s">
+        <v>193</v>
+      </c>
+      <c r="K21" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" ht="150" hidden="1">
+      <c r="A22" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C22" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G22" s="8"/>
+      <c r="H22" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I22" s="8"/>
+      <c r="J22" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="K22" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" ht="30">
+      <c r="A23" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" t="s">
+        <v>176</v>
+      </c>
+      <c r="H23" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J23" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="K23" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" ht="30">
+      <c r="A24" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>115</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E24" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F24" t="s">
+        <v>194</v>
+      </c>
+      <c r="H24" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J24" s="5" t="s">
+        <v>183</v>
+      </c>
+      <c r="K24" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" ht="30" hidden="1">
+      <c r="A25" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F25" s="11" t="s">
+        <v>177</v>
+      </c>
+      <c r="G25" s="8"/>
+      <c r="H25" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I25" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J25" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="K25" s="8"/>
+    </row>
+    <row r="26" spans="1:11" ht="30" hidden="1">
+      <c r="A26" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="G26" s="8"/>
+      <c r="H26" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I26" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J26" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="K26" s="8"/>
+    </row>
+    <row r="27" spans="1:11" ht="90">
+      <c r="A27" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" t="s">
+        <v>179</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I27" t="s">
+        <v>57</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="K27" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="45" hidden="1">
+      <c r="A28" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="C28" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="I28" t="s">
+        <v>14</v>
+      </c>
+      <c r="J28" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="K28" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" ht="30" hidden="1">
+      <c r="A29" t="s">
+        <v>60</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E29" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I29" t="s">
+        <v>26</v>
+      </c>
+      <c r="J29" s="4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="30" hidden="1">
+      <c r="A30" t="s">
+        <v>64</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="E30" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" t="s">
+        <v>26</v>
+      </c>
+      <c r="J30" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" ht="90">
+      <c r="A31" t="s">
+        <v>66</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" t="s">
+        <v>179</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I31" t="s">
+        <v>68</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="K31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="75" hidden="1">
+      <c r="A32" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" t="s">
+        <v>196</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="I32" t="s">
+        <v>97</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="45" hidden="1">
+      <c r="A33" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="G33" s="8"/>
+      <c r="H33" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="I33" t="s">
+        <v>43</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>200</v>
+      </c>
+      <c r="K33" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="60">
+      <c r="A34" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" t="s">
+        <v>194</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I34" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J34" s="9" t="s">
+        <v>201</v>
+      </c>
+      <c r="K34" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" ht="60">
+      <c r="A35" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B35" s="5" t="s">
+        <v>79</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" t="s">
+        <v>176</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I35" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J35" s="9" t="s">
+        <v>202</v>
+      </c>
+      <c r="K35" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="45">
+      <c r="A36" t="s">
+        <v>74</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" t="s">
+        <v>179</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I36" t="s">
+        <v>72</v>
+      </c>
+      <c r="J36" s="9" t="s">
+        <v>203</v>
+      </c>
+      <c r="K36" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="30" hidden="1">
+      <c r="A37" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>177</v>
+      </c>
+      <c r="G37" s="8"/>
+      <c r="H37" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K37" s="8"/>
+    </row>
+    <row r="38" spans="1:11" ht="30" hidden="1">
+      <c r="A38" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E38" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I38" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J38" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="90">
+      <c r="A39" t="s">
+        <v>112</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>113</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" t="s">
+        <v>204</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I39" t="s">
+        <v>86</v>
+      </c>
+      <c r="J39" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="K39" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" ht="45" hidden="1">
+      <c r="A40" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C40" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="9" t="s">
+        <v>180</v>
+      </c>
+      <c r="G40" s="8"/>
+      <c r="H40" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="I40" t="s">
+        <v>116</v>
+      </c>
+      <c r="J40" s="4" t="s">
+        <v>184</v>
+      </c>
+      <c r="K40" s="8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="30">
+      <c r="A41" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B41" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D41" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F41" t="s">
+        <v>176</v>
+      </c>
+      <c r="H41" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="J41" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="K41" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" ht="30">
+      <c r="A42" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B42" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E42" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F42" t="s">
+        <v>176</v>
+      </c>
+      <c r="H42" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="J42" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="K42" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" hidden="1">
+      <c r="A43" t="s">
+        <v>87</v>
+      </c>
+      <c r="B43" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" t="s">
+        <v>35</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>178</v>
+      </c>
+      <c r="E43" t="s">
+        <v>32</v>
+      </c>
+      <c r="H43"/>
+      <c r="J43" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" hidden="1">
+      <c r="A44" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C44" t="s">
+        <v>35</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="E44" t="s">
+        <v>32</v>
+      </c>
+      <c r="H44"/>
+      <c r="J44" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:L44">
+    <filterColumn colId="2">
+      <filters>
+        <filter val="1PDECORATOR"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Removed un-wanted API calls and fixed validations.
</commit_message>
<xml_diff>
--- a/src/test/test-data/DecoratorTestData.xlsx
+++ b/src/test/test-data/DecoratorTestData.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Decorator!$A$1:$L$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Decorator!$A$1:$L$29</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NewUsers!$A$1:$L$44</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1169" uniqueCount="233">
   <si>
     <t>API</t>
   </si>
@@ -718,12 +718,6 @@
     <t>status=200||notify.__typename=POST_CREATED||notify.post.id=(OPQA-360_id)||notify.post.issuerProfile.truid=(SYS_USER2)</t>
   </si>
   <si>
-    <t>status=200||notify.__typename=POST_CREATED||notify.post.id=(OPQA-360_id)||notify.issuerProfile.truid=(SYS_USER2)</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER2)</t>
-  </si>
-  <si>
     <t>/follow/user/(SYS_USER2)/following/(SYS_USER3)</t>
   </si>
   <si>
@@ -739,15 +733,9 @@
     <t>X-1P-User=(SYS_USER3)</t>
   </si>
   <si>
-    <t>status=200||notify.__typename=AppreciationEvent||notify.profilesByGroup.profile.truid=(SYS_USER3)||notify.profilesByGroup.profile.truid=(SYS_USER1)||notify.publicationRef.comment.id=(OPQA-236_comments.id)||notify.publicationRef.comment.content=Notification Test</t>
-  </si>
-  <si>
     <t>x-1p-user=(SYS_USER3)</t>
   </si>
   <si>
-    <t>status=200||notify.__typename=AppreciationEvent||notify.profilesByGroup.profile.truid=(SYS_USER3)||notify.profilesByGroup.profile.truid=(SYS_USER1)||notify.publicationRef.comment.id=(OPQA-385_comments.id)||notify.publicationRef.comment.content=Notification Test (ddMMMyyyy_HHmmss)</t>
-  </si>
-  <si>
     <t>X-1P-User=(SYS_USER4)||Content-Type=application/json</t>
   </si>
   <si>
@@ -757,25 +745,35 @@
     <t>X-1P-User=(SYS_USER4)</t>
   </si>
   <si>
-    <t>status=200||notify.__typename=AppreciationEvent||notify.issuer=(SYS_USER3)||notify.issuer=(SYS_USER1)||notify.publicationRef.comment.post.id=(OPQA-360_id)||notify.publicationRef.comment.post.title=Creating Post For API Notification Testing</t>
-  </si>
-  <si>
     <t>status=200||notify.__typename=PUBLIC_WATCHLIST||notify.issuerProfile.truid=(SYS_USER3)||notify.publication.containerId=(OPQA-312_containerId)||notify.action=EDIT_PERMISSIONS_IN_WATCHLIST</t>
   </si>
   <si>
-    <t>status=200||notify.cause=MyDocumentComment||notify.issuer=(SYS_USER4)||notify.comments.content=Notification Test (ddMMMyyyy_HHmmss)||notify.id=(OPQA-360_id)</t>
-  </si>
-  <si>
-    <t>status=200||notify.cause=WatchedDocumentComment||notify.issuerProfile.truid=(SYS_USER4)||notify.comments.content=Notification Test (ddMMMyyyy_HHmmss)||notify.id=(OPQA-360_id)</t>
-  </si>
-  <si>
-    <t>status=200||notify.__typename=DocumentCommentPost||notify.issuerProfile.truid=(SYS_USER4)||notify.comments.content=Notification Test (ddMMMyyyy_HHmmss)||notify.id=(OPQA-360_id)</t>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>FAIL</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=AppreciationEvent_V2||notify.issuer=(SYS_USER3)||notify.issuer=(SYS_USER1)||notify.publicationRef.post.id=(OPQA-360_id)||notify.publicationRef.post.title=Creating Post For API Notification Testing</t>
+  </si>
+  <si>
+    <t>status=200||notify.cause=WatchedDocumentComment||notify.issuerProfile.truid=(SYS_USER4)||notify.comments.content=Notification Test (ddMMMyyyy_HHmmss)||notify.post.id=(OPQA-360_id)</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=DocumentCommentPost||notify.issuerProfile.truid=(SYS_USER4)||notify.comments.content=Notification Test (ddMMMyyyy_HHmmss)||notify.post.id=(OPQA-360_id)</t>
+  </si>
+  <si>
+    <t>status=200||notify.cause=MyDocumentComment||notify.issuer=(SYS_USER4)||notify.comments.content=Notification Test (ddMMMyyyy_HHmmss)||notify.post.id=(OPQA-360_id)</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=AppreciationEvent_V2||notify.profilesByGroup.profile.truid=(SYS_USER3)||notify.profilesByGroup.profile.truid=(SYS_USER1)||notify.publicationRef.post.id=(OPQA-385_comments.id)||notify.publicationRef.post.content=Notification Test (ddMMMyyyy_HHmmss)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
   <fonts count="3">
     <font>
       <sz val="11"/>
@@ -1183,26 +1181,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L41"/>
+    <sheetView tabSelected="1" topLeftCell="H19" workbookViewId="0">
+      <selection activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="73" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="87.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="47.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="52.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="61.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="65.7109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="73.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="87.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="52.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="5" width="61.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="65.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -1271,6 +1269,9 @@
       <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
+      <c r="L2" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="3" spans="1:12" ht="30">
       <c r="A3" s="4" t="s">
@@ -1288,15 +1289,20 @@
       <c r="E3" s="1" t="s">
         <v>23</v>
       </c>
+      <c r="F3"/>
       <c r="G3" s="5" t="s">
         <v>119</v>
       </c>
       <c r="H3"/>
+      <c r="I3"/>
       <c r="J3" s="4" t="s">
         <v>12</v>
       </c>
       <c r="K3" s="1" t="s">
         <v>24</v>
+      </c>
+      <c r="L3" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30">
@@ -1323,6 +1329,9 @@
         <v>36</v>
       </c>
       <c r="K4" s="1"/>
+      <c r="L4" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
@@ -1343,6 +1352,7 @@
       <c r="F5" t="s">
         <v>212</v>
       </c>
+      <c r="G5"/>
       <c r="H5" s="5" t="s">
         <v>136</v>
       </c>
@@ -1354,6 +1364,9 @@
       </c>
       <c r="K5" t="s">
         <v>137</v>
+      </c>
+      <c r="L5" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1367,7 +1380,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
@@ -1375,10 +1388,14 @@
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
       <c r="H6" s="4"/>
+      <c r="I6"/>
       <c r="J6" s="5" t="s">
         <v>36</v>
       </c>
       <c r="K6" s="1"/>
+      <c r="L6" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="7" spans="1:12" ht="45">
       <c r="A7" s="8" t="s">
@@ -1399,6 +1416,7 @@
       <c r="F7" t="s">
         <v>209</v>
       </c>
+      <c r="G7"/>
       <c r="H7" s="5" t="s">
         <v>136</v>
       </c>
@@ -1406,10 +1424,13 @@
         <v>39</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="K7" t="s">
         <v>137</v>
+      </c>
+      <c r="L7" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="120">
@@ -1429,7 +1450,7 @@
         <v>13</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="4" t="s">
@@ -1442,6 +1463,9 @@
       <c r="K8" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="L8" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="9" spans="1:12" ht="45">
       <c r="A9" s="5" t="s">
@@ -1462,6 +1486,7 @@
       <c r="F9" t="s">
         <v>212</v>
       </c>
+      <c r="G9"/>
       <c r="H9" s="5" t="s">
         <v>136</v>
       </c>
@@ -1469,10 +1494,13 @@
         <v>92</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="K9" t="s">
         <v>137</v>
+      </c>
+      <c r="L9" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="10" spans="1:12" ht="60">
@@ -1492,7 +1520,7 @@
         <v>101</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="4" t="s">
@@ -1505,6 +1533,9 @@
         <v>12</v>
       </c>
       <c r="K10" s="1"/>
+      <c r="L10" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="11" spans="1:12" ht="60">
       <c r="A11" s="4" t="s">
@@ -1523,7 +1554,7 @@
         <v>101</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="4" t="s">
@@ -1536,6 +1567,9 @@
         <v>12</v>
       </c>
       <c r="K11" s="1"/>
+      <c r="L11" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="12" spans="1:12" ht="45">
       <c r="A12" s="5" t="s">
@@ -1556,6 +1590,7 @@
       <c r="F12" t="s">
         <v>212</v>
       </c>
+      <c r="G12"/>
       <c r="H12" s="5" t="s">
         <v>136</v>
       </c>
@@ -1563,10 +1598,13 @@
         <v>92</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="K12" t="s">
         <v>137</v>
+      </c>
+      <c r="L12" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="13" spans="1:12" ht="150">
@@ -1599,6 +1637,9 @@
       <c r="K13" s="10" t="s">
         <v>46</v>
       </c>
+      <c r="L13" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" s="8" t="s">
@@ -1619,6 +1660,7 @@
       <c r="F14" t="s">
         <v>209</v>
       </c>
+      <c r="G14"/>
       <c r="H14" s="5" t="s">
         <v>136</v>
       </c>
@@ -1631,42 +1673,47 @@
       <c r="K14" t="s">
         <v>137</v>
       </c>
+      <c r="L14" t="s">
+        <v>226</v>
+      </c>
     </row>
     <row r="15" spans="1:12" ht="30">
       <c r="A15" s="8" t="s">
-        <v>114</v>
+        <v>49</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>115</v>
-      </c>
-      <c r="C15" s="1" t="s">
-        <v>134</v>
+        <v>51</v>
+      </c>
+      <c r="C15" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F15" t="s">
-        <v>222</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>136</v>
+        <v>52</v>
+      </c>
+      <c r="E15" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F15" s="11" t="s">
+        <v>210</v>
+      </c>
+      <c r="G15" s="8"/>
+      <c r="H15" s="11" t="s">
+        <v>50</v>
       </c>
       <c r="I15" s="8" t="s">
         <v>43</v>
       </c>
-      <c r="J15" s="5" t="s">
-        <v>216</v>
-      </c>
-      <c r="K15" t="s">
-        <v>137</v>
+      <c r="J15" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="K15" s="8"/>
+      <c r="L15" t="s">
+        <v>226</v>
       </c>
     </row>
     <row r="16" spans="1:12" ht="30">
       <c r="A16" s="8" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="B16" s="5" t="s">
         <v>51</v>
@@ -1680,8 +1727,8 @@
       <c r="E16" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>210</v>
+      <c r="F16" s="9" t="s">
+        <v>218</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="11" t="s">
@@ -1691,170 +1738,197 @@
         <v>43</v>
       </c>
       <c r="J16" s="9" t="s">
-        <v>53</v>
+        <v>91</v>
       </c>
       <c r="K16" s="8"/>
-    </row>
-    <row r="17" spans="1:11" ht="30">
-      <c r="A17" s="8" t="s">
-        <v>54</v>
+      <c r="L16" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" ht="60">
+      <c r="A17" s="5" t="s">
+        <v>55</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="C17" s="10" t="s">
-        <v>27</v>
+        <v>56</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="E17" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F17" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="G17" s="8"/>
-      <c r="H17" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="I17" s="8" t="s">
-        <v>43</v>
-      </c>
-      <c r="J17" s="9" t="s">
-        <v>91</v>
-      </c>
-      <c r="K17" s="8"/>
-    </row>
-    <row r="18" spans="1:11" ht="75">
+        <v>135</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F17" t="s">
+        <v>212</v>
+      </c>
+      <c r="G17"/>
+      <c r="H17" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="I17" t="s">
+        <v>57</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>228</v>
+      </c>
+      <c r="K17" t="s">
+        <v>137</v>
+      </c>
+      <c r="L17" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" ht="75">
       <c r="A18" s="5" t="s">
-        <v>55</v>
+        <v>100</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>135</v>
+        <v>70</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+      <c r="D18" s="7" t="s">
+        <v>95</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F18" t="s">
-        <v>212</v>
-      </c>
+        <v>221</v>
+      </c>
+      <c r="G18"/>
       <c r="H18" s="5" t="s">
-        <v>136</v>
+        <v>96</v>
       </c>
       <c r="I18" t="s">
-        <v>57</v>
+        <v>97</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>229</v>
-      </c>
-      <c r="K18" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="19" spans="1:11" ht="45">
+        <v>12</v>
+      </c>
+      <c r="K18"/>
+      <c r="L18" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" ht="45">
       <c r="A19" s="8" t="s">
-        <v>26</v>
+        <v>72</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>207</v>
-      </c>
-      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+      <c r="C19" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
       <c r="G19" s="8"/>
-      <c r="H19" s="4" t="s">
-        <v>142</v>
+      <c r="H19" s="9" t="s">
+        <v>143</v>
       </c>
       <c r="I19" t="s">
-        <v>14</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="K19" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="J19" s="9" t="s">
+        <v>223</v>
+      </c>
+      <c r="K19" s="10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="20" spans="1:11" ht="30">
-      <c r="A20" t="s">
-        <v>60</v>
+      <c r="L19" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" ht="45">
+      <c r="A20" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C20" t="s">
-        <v>27</v>
+        <v>77</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="D20" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E20" t="s">
-        <v>13</v>
-      </c>
-      <c r="F20" s="9" t="s">
-        <v>210</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" t="s">
+        <v>220</v>
+      </c>
+      <c r="G20"/>
       <c r="H20" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I20" t="s">
-        <v>26</v>
-      </c>
-      <c r="J20" s="4" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="21" spans="1:11" ht="30">
-      <c r="A21" t="s">
-        <v>64</v>
+        <v>136</v>
+      </c>
+      <c r="I20" s="8" t="s">
+        <v>132</v>
+      </c>
+      <c r="J20" s="9" t="s">
+        <v>229</v>
+      </c>
+      <c r="K20" t="s">
+        <v>137</v>
+      </c>
+      <c r="L20" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" ht="45">
+      <c r="A21" s="8" t="s">
+        <v>78</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="C21" t="s">
-        <v>27</v>
+        <v>79</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="E21" t="s">
-        <v>13</v>
-      </c>
-      <c r="F21" s="9" t="s">
-        <v>220</v>
-      </c>
+        <v>135</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F21" t="s">
+        <v>209</v>
+      </c>
+      <c r="G21"/>
       <c r="H21" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I21" t="s">
-        <v>26</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="22" spans="1:11" ht="75">
+        <v>136</v>
+      </c>
+      <c r="I21" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J21" s="9" t="s">
+        <v>230</v>
+      </c>
+      <c r="K21" t="s">
+        <v>137</v>
+      </c>
+      <c r="L21" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" ht="45">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>74</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>67</v>
+        <v>75</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>134</v>
@@ -1868,87 +1942,97 @@
       <c r="F22" t="s">
         <v>212</v>
       </c>
+      <c r="G22"/>
       <c r="H22" s="5" t="s">
         <v>136</v>
       </c>
       <c r="I22" t="s">
-        <v>68</v>
-      </c>
-      <c r="J22" s="5" t="s">
-        <v>223</v>
+        <v>72</v>
+      </c>
+      <c r="J22" s="9" t="s">
+        <v>231</v>
       </c>
       <c r="K22" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="23" spans="1:11" ht="75">
-      <c r="A23" s="5" t="s">
-        <v>100</v>
+      <c r="L22" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" ht="30">
+      <c r="A23" s="8" t="s">
+        <v>80</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="C23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="7" t="s">
-        <v>95</v>
-      </c>
-      <c r="E23" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F23" t="s">
-        <v>224</v>
-      </c>
-      <c r="H23" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="I23" t="s">
-        <v>97</v>
-      </c>
-      <c r="J23" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="24" spans="1:11" ht="45">
+        <v>83</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="9" t="s">
+        <v>210</v>
+      </c>
+      <c r="G23" s="8"/>
+      <c r="H23" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I23" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J23" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="K23" s="8"/>
+      <c r="L23" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" ht="30">
       <c r="A24" s="8" t="s">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D24" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E24" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="E24" t="s">
         <v>13</v>
       </c>
       <c r="F24" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="G24"/>
+      <c r="H24" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="I24" s="8" t="s">
+        <v>72</v>
+      </c>
+      <c r="J24" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="K24"/>
+      <c r="L24" t="s">
         <v>226</v>
       </c>
-      <c r="G24" s="8"/>
-      <c r="H24" s="9" t="s">
-        <v>143</v>
-      </c>
-      <c r="I24" t="s">
-        <v>43</v>
-      </c>
-      <c r="J24" s="9" t="s">
-        <v>227</v>
-      </c>
-      <c r="K24" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="25" spans="1:11" ht="45">
-      <c r="A25" s="8" t="s">
-        <v>76</v>
+    </row>
+    <row r="25" spans="1:12" ht="75">
+      <c r="A25" t="s">
+        <v>112</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>77</v>
+        <v>113</v>
       </c>
       <c r="C25" s="1" t="s">
         <v>134</v>
@@ -1960,13 +2044,14 @@
         <v>13</v>
       </c>
       <c r="F25" t="s">
-        <v>222</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="G25"/>
       <c r="H25" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="I25" s="8" t="s">
-        <v>132</v>
+      <c r="I25" t="s">
+        <v>86</v>
       </c>
       <c r="J25" s="9" t="s">
         <v>232</v>
@@ -1974,13 +2059,16 @@
       <c r="K25" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="26" spans="1:11" ht="45">
-      <c r="A26" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="B26" s="5" t="s">
-        <v>79</v>
+      <c r="L25" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="30">
+      <c r="A26" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>146</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>134</v>
@@ -1994,25 +2082,27 @@
       <c r="F26" t="s">
         <v>209</v>
       </c>
+      <c r="G26"/>
       <c r="H26" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="I26" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="J26" s="9" t="s">
-        <v>233</v>
+      <c r="I26"/>
+      <c r="J26" s="5" t="s">
+        <v>149</v>
       </c>
       <c r="K26" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="27" spans="1:11" ht="45">
-      <c r="A27" t="s">
-        <v>74</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>75</v>
+      <c r="L26" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" ht="30">
+      <c r="A27" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>148</v>
       </c>
       <c r="C27" s="1" t="s">
         <v>134</v>
@@ -2024,244 +2114,77 @@
         <v>13</v>
       </c>
       <c r="F27" t="s">
-        <v>212</v>
-      </c>
+        <v>209</v>
+      </c>
+      <c r="G27"/>
       <c r="H27" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="I27" t="s">
-        <v>72</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>231</v>
+      <c r="I27"/>
+      <c r="J27" s="5" t="s">
+        <v>150</v>
       </c>
       <c r="K27" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" ht="30">
-      <c r="A28" s="8" t="s">
-        <v>80</v>
+      <c r="L27" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12">
+      <c r="A28" t="s">
+        <v>87</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>27</v>
+        <v>88</v>
+      </c>
+      <c r="C28" t="s">
+        <v>35</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>81</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="G28" s="8"/>
-      <c r="H28" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="J28" s="9" t="s">
-        <v>82</v>
-      </c>
-      <c r="K28" s="8"/>
-    </row>
-    <row r="29" spans="1:11" ht="30">
-      <c r="A29" s="8" t="s">
-        <v>84</v>
+        <v>211</v>
+      </c>
+      <c r="E28" t="s">
+        <v>32</v>
+      </c>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="K28"/>
+      <c r="L28" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12">
+      <c r="A29" t="s">
+        <v>90</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>27</v>
+        <v>88</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>81</v>
+        <v>216</v>
       </c>
       <c r="E29" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" s="9" t="s">
-        <v>220</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="I29" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="J29" s="9" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="75">
-      <c r="A30" t="s">
-        <v>112</v>
-      </c>
-      <c r="B30" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D30" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E30" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F30" t="s">
-        <v>228</v>
-      </c>
-      <c r="H30" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="I30" t="s">
-        <v>86</v>
-      </c>
-      <c r="J30" s="9" t="s">
-        <v>225</v>
-      </c>
-      <c r="K30" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" ht="45">
-      <c r="A31" s="8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B31" s="5" t="s">
-        <v>125</v>
-      </c>
-      <c r="C31" t="s">
-        <v>27</v>
-      </c>
-      <c r="D31" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="G31" s="8"/>
-      <c r="H31" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="I31" t="s">
-        <v>116</v>
-      </c>
-      <c r="J31" s="4" t="s">
-        <v>217</v>
-      </c>
-      <c r="K31" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="32" spans="1:11" ht="30">
-      <c r="A32" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" t="s">
-        <v>209</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="K32" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="30">
-      <c r="A33" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" t="s">
-        <v>209</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="J33" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="K33" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
-      <c r="A34" t="s">
-        <v>87</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="E34" t="s">
         <v>32</v>
       </c>
-      <c r="H34"/>
-      <c r="J34" s="5" t="s">
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29" s="5" t="s">
         <v>89</v>
       </c>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" t="s">
-        <v>90</v>
-      </c>
-      <c r="B35" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C35" t="s">
-        <v>35</v>
-      </c>
-      <c r="D35" s="6" t="s">
-        <v>218</v>
-      </c>
-      <c r="E35" t="s">
-        <v>32</v>
-      </c>
-      <c r="H35"/>
-      <c r="J35" s="5" t="s">
-        <v>89</v>
+      <c r="K29"/>
+      <c r="L29" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>
@@ -2273,24 +2196,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L50"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L3" sqref="L3"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="73" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="87.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="47.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="52.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="61.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="65.7109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="73.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="87.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="52.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="5" width="61.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="65.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -3805,24 +3728,24 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:L44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+    <sheetView topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="73" style="5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="16" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="87.85546875" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="47.28515625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="52.85546875" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="61.85546875" style="5" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="65.7109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" customWidth="true" width="31.0" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="5" width="73.0" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="16.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="87.85546875" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="47.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="52.85546875" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="5" width="61.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" style="5" width="65.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">

</xml_diff>

<commit_message>
Created Batch Job Events for HPA Notification
</commit_message>
<xml_diff>
--- a/src/test/test-data/DecoratorTestData.xlsx
+++ b/src/test/test-data/DecoratorTestData.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Decorator!$A$1:$L$29</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Decorator!$A$1:$L$35</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NewUsers!$A$1:$L$44</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1140" uniqueCount="233">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="255">
   <si>
     <t>API</t>
   </si>
@@ -748,12 +748,6 @@
     <t>status=200||notify.__typename=PUBLIC_WATCHLIST||notify.issuerProfile.truid=(SYS_USER3)||notify.publication.containerId=(OPQA-312_containerId)||notify.action=EDIT_PERMISSIONS_IN_WATCHLIST</t>
   </si>
   <si>
-    <t>PASS</t>
-  </si>
-  <si>
-    <t>FAIL</t>
-  </si>
-  <si>
     <t>status=200||notify.__typename=AppreciationEvent_V2||notify.issuer=(SYS_USER3)||notify.issuer=(SYS_USER1)||notify.publicationRef.post.id=(OPQA-360_id)||notify.publicationRef.post.title=Creating Post For API Notification Testing</t>
   </si>
   <si>
@@ -766,7 +760,79 @@
     <t>status=200||notify.cause=MyDocumentComment||notify.issuer=(SYS_USER4)||notify.comments.content=Notification Test (ddMMMyyyy_HHmmss)||notify.post.id=(OPQA-360_id)</t>
   </si>
   <si>
-    <t>status=200||notify.__typename=AppreciationEvent_V2||notify.profilesByGroup.profile.truid=(SYS_USER3)||notify.profilesByGroup.profile.truid=(SYS_USER1)||notify.publicationRef.post.id=(OPQA-385_comments.id)||notify.publicationRef.post.content=Notification Test (ddMMMyyyy_HHmmss)</t>
+    <t>status=200||notify.__typename=AppreciationEvent_V2||notify.issuer=(SYS_USER3)||notify.issuer=(SYS_USER1)||notify.publicationRef.post.id=(OPQA-385_comments.id)||notify.publicationRef.post.content=Notification Test (ddMMMyyyy_HHmmss)</t>
+  </si>
+  <si>
+    <t>status=200||userId=(SYS_USER4)||found=true</t>
+  </si>
+  <si>
+    <t>OPQA-360_1</t>
+  </si>
+  <si>
+    <t>{"targetType":"posts","targetId":"(OPQA-360_1_id)","content":"Adding Comment on post for Notification Test (ddMMMyyyy_HHmmss)"}</t>
+  </si>
+  <si>
+    <t>OPQA-385_1</t>
+  </si>
+  <si>
+    <t>OPQA-385_2</t>
+  </si>
+  <si>
+    <t>{"targetType":"posts","targetId":"(OPQA-360_1_id)","content":"Adding Comment on post for HPA Notification Test (ddMMMyyyy_HHmmss)"}</t>
+  </si>
+  <si>
+    <t>Verify that user receives a notification if someone commented of his commented post</t>
+  </si>
+  <si>
+    <t>OPQA-360_2</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER4)||comments.targetType=Post||comments.targetId=(OPQA-360_2_id)||comments.content=Notification Test</t>
+  </si>
+  <si>
+    <t>{"targetType":"posts","targetId":"(OPQA-360_2_id)","content":"Adding Comment on post for Notification Test (ddMMMyyyy_HHmmss)"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER4)||comments.targetType=Post||comments.targetId=(OPQA-360_2_id)||comments.content=HPA Notification Test</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=authoringTargetComments||notify.issuerProfile.truid=(SYS_USER3)||notify.targetId=(OPQA-360_2_id)</t>
+  </si>
+  <si>
+    <t>OPQA-385_3</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER3)||comments.targetType=Post||comments.targetId=(OPQA-360_1_id)||comments.content=Notification Test</t>
+  </si>
+  <si>
+    <t>/appreciation/appreciate/Comment/(OPQA-385_3_comments.id)</t>
+  </si>
+  <si>
+    <t>status=200||hasAppreciated=UP||targetType=Comment||appreciateCount=1||targetId=(OPQA-385_3_comments.id)</t>
+  </si>
+  <si>
+    <t>Verify that user receives notifications if someone he is following liked a post comment.</t>
+  </si>
+  <si>
+    <t>Verify that user receives notifications if someone he is following liked the post.</t>
+  </si>
+  <si>
+    <t>Verify that the user is able to appreciate the posts of others.</t>
+  </si>
+  <si>
+    <t>/appreciation/appreciate/posts/(OPQA-360_1_id)</t>
+  </si>
+  <si>
+    <t>status=200||hasAppreciated=UP||targetType=posts||targetId=(OPQA-360_1_id)</t>
+  </si>
+  <si>
+    <t>OPQA-4140</t>
+  </si>
+  <si>
+    <t>OPQA-4141</t>
+  </si>
+  <si>
+    <t>OPQA-4143</t>
   </si>
 </sst>
 </file>
@@ -848,7 +914,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -884,6 +950,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1180,10 +1249,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H19" workbookViewId="0">
-      <selection activeCell="L29" sqref="L29"/>
+    <sheetView tabSelected="1" topLeftCell="H27" workbookViewId="0">
+      <selection activeCell="M31" sqref="M31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1268,9 +1337,6 @@
       <c r="K2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="L2" t="s">
-        <v>226</v>
-      </c>
     </row>
     <row r="3" spans="1:12" ht="30">
       <c r="A3" s="4" t="s">
@@ -1297,9 +1363,6 @@
       </c>
       <c r="K3" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="L3" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="4" spans="1:12" ht="30">
@@ -1326,9 +1389,6 @@
         <v>36</v>
       </c>
       <c r="K4" s="1"/>
-      <c r="L4" t="s">
-        <v>226</v>
-      </c>
     </row>
     <row r="5" spans="1:12" ht="30">
       <c r="A5" t="s">
@@ -1360,9 +1420,6 @@
       </c>
       <c r="K5" t="s">
         <v>137</v>
-      </c>
-      <c r="L5" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="6" spans="1:12">
@@ -1388,9 +1445,6 @@
         <v>36</v>
       </c>
       <c r="K6" s="1"/>
-      <c r="L6" t="s">
-        <v>226</v>
-      </c>
     </row>
     <row r="7" spans="1:12" ht="45">
       <c r="A7" s="8" t="s">
@@ -1423,9 +1477,6 @@
       <c r="K7" t="s">
         <v>137</v>
       </c>
-      <c r="L7" t="s">
-        <v>226</v>
-      </c>
     </row>
     <row r="8" spans="1:12" ht="120">
       <c r="A8" s="5" t="s">
@@ -1457,9 +1508,6 @@
       <c r="K8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="L8" t="s">
-        <v>226</v>
-      </c>
     </row>
     <row r="9" spans="1:12" ht="45">
       <c r="A9" s="5" t="s">
@@ -1492,9 +1540,6 @@
       <c r="K9" t="s">
         <v>137</v>
       </c>
-      <c r="L9" t="s">
-        <v>226</v>
-      </c>
     </row>
     <row r="10" spans="1:12" ht="60">
       <c r="A10" s="4" t="s">
@@ -1526,9 +1571,6 @@
         <v>12</v>
       </c>
       <c r="K10" s="1"/>
-      <c r="L10" t="s">
-        <v>226</v>
-      </c>
     </row>
     <row r="11" spans="1:12" ht="60">
       <c r="A11" s="4" t="s">
@@ -1560,9 +1602,6 @@
         <v>12</v>
       </c>
       <c r="K11" s="1"/>
-      <c r="L11" t="s">
-        <v>226</v>
-      </c>
     </row>
     <row r="12" spans="1:12" ht="45">
       <c r="A12" s="5" t="s">
@@ -1595,9 +1634,6 @@
       <c r="K12" t="s">
         <v>137</v>
       </c>
-      <c r="L12" t="s">
-        <v>226</v>
-      </c>
     </row>
     <row r="13" spans="1:12" ht="150">
       <c r="A13" s="8" t="s">
@@ -1629,9 +1665,6 @@
       <c r="K13" s="10" t="s">
         <v>46</v>
       </c>
-      <c r="L13" t="s">
-        <v>226</v>
-      </c>
     </row>
     <row r="14" spans="1:12" ht="30">
       <c r="A14" s="8" t="s">
@@ -1664,9 +1697,6 @@
       <c r="K14" t="s">
         <v>137</v>
       </c>
-      <c r="L14" t="s">
-        <v>226</v>
-      </c>
     </row>
     <row r="15" spans="1:12" ht="30">
       <c r="A15" s="8" t="s">
@@ -1698,9 +1728,6 @@
         <v>53</v>
       </c>
       <c r="K15" s="8"/>
-      <c r="L15" t="s">
-        <v>226</v>
-      </c>
     </row>
     <row r="16" spans="1:12" ht="30">
       <c r="A16" s="8" t="s">
@@ -1732,11 +1759,8 @@
         <v>91</v>
       </c>
       <c r="K16" s="8"/>
-      <c r="L16" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="60">
+    </row>
+    <row r="17" spans="1:11" ht="60">
       <c r="A17" s="5" t="s">
         <v>55</v>
       </c>
@@ -1762,16 +1786,13 @@
         <v>57</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="K17" t="s">
         <v>137</v>
       </c>
-      <c r="L17" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" ht="75">
+    </row>
+    <row r="18" spans="1:11" ht="75">
       <c r="A18" s="5" t="s">
         <v>100</v>
       </c>
@@ -1799,11 +1820,8 @@
       <c r="J18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="L18" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" ht="45">
+    </row>
+    <row r="19" spans="1:11" ht="45">
       <c r="A19" s="8" t="s">
         <v>72</v>
       </c>
@@ -1835,11 +1853,8 @@
       <c r="K19" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="L19" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" ht="45">
+    </row>
+    <row r="20" spans="1:11" ht="45">
       <c r="A20" s="8" t="s">
         <v>76</v>
       </c>
@@ -1865,16 +1880,13 @@
         <v>132</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="K20" t="s">
         <v>137</v>
       </c>
-      <c r="L20" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" ht="45">
+    </row>
+    <row r="21" spans="1:11" ht="45">
       <c r="A21" s="8" t="s">
         <v>78</v>
       </c>
@@ -1900,16 +1912,13 @@
         <v>72</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="K21" t="s">
         <v>137</v>
       </c>
-      <c r="L21" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" ht="45">
+    </row>
+    <row r="22" spans="1:11" ht="45">
       <c r="A22" t="s">
         <v>74</v>
       </c>
@@ -1935,16 +1944,13 @@
         <v>72</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="K22" t="s">
         <v>137</v>
       </c>
-      <c r="L22" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" ht="30">
+    </row>
+    <row r="23" spans="1:11" ht="30">
       <c r="A23" s="8" t="s">
         <v>80</v>
       </c>
@@ -1974,11 +1980,8 @@
         <v>82</v>
       </c>
       <c r="K23" s="8"/>
-      <c r="L23" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" ht="30">
+    </row>
+    <row r="24" spans="1:11" ht="30">
       <c r="A24" s="8" t="s">
         <v>84</v>
       </c>
@@ -2006,11 +2009,8 @@
       <c r="J24" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="L24" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" ht="75">
+    </row>
+    <row r="25" spans="1:11" ht="75">
       <c r="A25" t="s">
         <v>112</v>
       </c>
@@ -2036,122 +2036,420 @@
         <v>86</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="K25" t="s">
         <v>137</v>
       </c>
-      <c r="L25" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="30">
-      <c r="A26" s="12" t="s">
+    </row>
+    <row r="26" spans="1:11" ht="150">
+      <c r="A26" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C26" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E26" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="G26" s="8"/>
+      <c r="H26" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I26" s="8"/>
+      <c r="J26" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="K26" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="45">
+      <c r="A27" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="G27" s="8"/>
+      <c r="H27" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="I27" t="s">
+        <v>232</v>
+      </c>
+      <c r="J27" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="K27" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" ht="30">
+      <c r="A28" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F28" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="G28" s="8"/>
+      <c r="H28" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="I28" s="8" t="s">
+        <v>243</v>
+      </c>
+      <c r="J28" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="K28" s="8"/>
+    </row>
+    <row r="29" spans="1:11" ht="30">
+      <c r="A29" s="8" t="s">
+        <v>253</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>247</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F29" t="s">
+        <v>209</v>
+      </c>
+      <c r="H29" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="J29" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K29" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="30">
+      <c r="A30" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="B30" s="16" t="s">
+        <v>249</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="E30" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F30" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="G30" s="8"/>
+      <c r="H30" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I30" s="8" t="s">
+        <v>232</v>
+      </c>
+      <c r="J30" s="9" t="s">
+        <v>251</v>
+      </c>
+      <c r="K30" s="8"/>
+    </row>
+    <row r="31" spans="1:11" ht="30">
+      <c r="A31" s="8" t="s">
+        <v>254</v>
+      </c>
+      <c r="B31" s="5" t="s">
+        <v>248</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E31" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F31" t="s">
+        <v>209</v>
+      </c>
+      <c r="H31" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="J31" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K31" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="30">
+      <c r="A32" s="12" t="s">
         <v>145</v>
       </c>
-      <c r="B26" s="13" t="s">
+      <c r="B32" s="13" t="s">
         <v>146</v>
       </c>
-      <c r="C26" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D32" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E26" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="E32" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" t="s">
         <v>209</v>
       </c>
-      <c r="H26" s="5" t="s">
+      <c r="H32" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="J26" s="5" t="s">
+      <c r="J32" s="5" t="s">
         <v>149</v>
       </c>
-      <c r="K26" t="s">
+      <c r="K32" t="s">
         <v>137</v>
       </c>
-      <c r="L26" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" ht="30">
-      <c r="A27" s="12" t="s">
+    </row>
+    <row r="33" spans="1:11" ht="30">
+      <c r="A33" s="12" t="s">
         <v>147</v>
       </c>
-      <c r="B27" s="13" t="s">
+      <c r="B33" s="13" t="s">
         <v>148</v>
       </c>
-      <c r="C27" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D33" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E27" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="E33" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" t="s">
         <v>209</v>
       </c>
-      <c r="H27" s="5" t="s">
+      <c r="H33" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="J27" s="5" t="s">
+      <c r="J33" s="5" t="s">
         <v>150</v>
       </c>
-      <c r="K27" t="s">
+      <c r="K33" t="s">
         <v>137</v>
       </c>
-      <c r="L27" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12">
-      <c r="A28" t="s">
+    </row>
+    <row r="34" spans="1:11">
+      <c r="A34" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B34" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C34" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D34" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="E28" t="s">
+      <c r="E34" t="s">
         <v>32</v>
       </c>
-      <c r="H28"/>
-      <c r="J28" s="5" t="s">
+      <c r="H34"/>
+      <c r="J34" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="L28" t="s">
-        <v>226</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12">
-      <c r="A29" t="s">
+    </row>
+    <row r="35" spans="1:11">
+      <c r="A35" t="s">
         <v>90</v>
       </c>
-      <c r="B29" s="5" t="s">
+      <c r="B35" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C35" t="s">
         <v>35</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D35" s="6" t="s">
         <v>216</v>
       </c>
-      <c r="E29" t="s">
+      <c r="E35" t="s">
         <v>32</v>
       </c>
-      <c r="H29"/>
-      <c r="J29" s="5" t="s">
+      <c r="H35"/>
+      <c r="J35" s="5" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="150">
+      <c r="A36" s="8" t="s">
+        <v>238</v>
+      </c>
+      <c r="B36" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C36" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E36" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F36" s="9" t="s">
+        <v>222</v>
+      </c>
+      <c r="G36" s="8"/>
+      <c r="H36" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="I36" s="8"/>
+      <c r="J36" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="K36" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="45">
+      <c r="A37" s="8" t="s">
+        <v>234</v>
+      </c>
+      <c r="B37" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E37" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F37" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="G37" s="8"/>
+      <c r="H37" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="I37" t="s">
+        <v>238</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>239</v>
+      </c>
+      <c r="K37" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" ht="45">
+      <c r="A38" s="8" t="s">
+        <v>235</v>
+      </c>
+      <c r="B38" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C38" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E38" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="G38" s="8"/>
+      <c r="H38" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="I38" t="s">
+        <v>43</v>
+      </c>
+      <c r="J38" s="9" t="s">
+        <v>241</v>
+      </c>
+      <c r="K38" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" ht="30">
+      <c r="A39" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="B39" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E39" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" t="s">
+        <v>212</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>242</v>
+      </c>
+      <c r="K39" t="s">
+        <v>137</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added SearchV4 in testng.xml and modified Batch job related test cases.
</commit_message>
<xml_diff>
--- a/src/test/test-data/DecoratorTestData.xlsx
+++ b/src/test/test-data/DecoratorTestData.xlsx
@@ -13,7 +13,7 @@
     <sheet name="Sheet1" sheetId="5" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Decorator!$A$1:$L$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Decorator!$A$1:$L$34</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">NewUsers!$A$1:$L$44</definedName>
   </definedNames>
   <calcPr calcId="125725"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1206" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1235" uniqueCount="276">
   <si>
     <t>API</t>
   </si>
@@ -697,9 +697,6 @@
     <t>status=200||notify.__typename=FOLLOW||notify.issuerProfile.truid=(SYS_USER1)</t>
   </si>
   <si>
-    <t>X-1P-User=(SYS_USER1)</t>
-  </si>
-  <si>
     <t>X-1P-User=(SYS_USER1)||Content-Type=application/json</t>
   </si>
   <si>
@@ -727,78 +724,36 @@
     <t>X-1P-User=(SYS_USER3)||Content-Type=application/json</t>
   </si>
   <si>
-    <t>status=200||notify.__typename==PUBLIC_WATCHLIST||notify.issuerProfile.truid=(SYS_USER3)||notify.publication.containerId=(OPQA-312_containerId)||notify.action=CREATE_WATCHLIST</t>
-  </si>
-  <si>
-    <t>X-1P-User=(SYS_USER3)</t>
-  </si>
-  <si>
-    <t>x-1p-user=(SYS_USER3)</t>
-  </si>
-  <si>
     <t>X-1P-User=(SYS_USER4)||Content-Type=application/json</t>
   </si>
   <si>
     <t>status=200||comments.userId=(SYS_USER4)||comments.targetType=Post||comments.targetId=(OPQA-360_id)||comments.content=Notification Test</t>
   </si>
   <si>
-    <t>X-1P-User=(SYS_USER4)</t>
-  </si>
-  <si>
-    <t>status=200||notify.__typename=PUBLIC_WATCHLIST||notify.issuerProfile.truid=(SYS_USER3)||notify.publication.containerId=(OPQA-312_containerId)||notify.action=EDIT_PERMISSIONS_IN_WATCHLIST</t>
-  </si>
-  <si>
     <t>status=200||notify.__typename=AppreciationEvent_V2||notify.issuer=(SYS_USER3)||notify.issuer=(SYS_USER1)||notify.publicationRef.post.id=(OPQA-360_id)||notify.publicationRef.post.title=Creating Post For API Notification Testing</t>
   </si>
   <si>
-    <t>status=200||notify.cause=WatchedDocumentComment||notify.issuerProfile.truid=(SYS_USER4)||notify.comments.content=Notification Test (ddMMMyyyy_HHmmss)||notify.post.id=(OPQA-360_id)</t>
-  </si>
-  <si>
     <t>status=200||notify.__typename=DocumentCommentPost||notify.issuerProfile.truid=(SYS_USER4)||notify.comments.content=Notification Test (ddMMMyyyy_HHmmss)||notify.post.id=(OPQA-360_id)</t>
   </si>
   <si>
     <t>status=200||notify.cause=MyDocumentComment||notify.issuer=(SYS_USER4)||notify.comments.content=Notification Test (ddMMMyyyy_HHmmss)||notify.post.id=(OPQA-360_id)</t>
   </si>
   <si>
-    <t>status=200||notify.__typename=AppreciationEvent_V2||notify.issuer=(SYS_USER3)||notify.issuer=(SYS_USER1)||notify.publicationRef.post.id=(OPQA-385_comments.id)||notify.publicationRef.post.content=Notification Test (ddMMMyyyy_HHmmss)</t>
-  </si>
-  <si>
     <t>status=200||userId=(SYS_USER4)||found=true</t>
   </si>
   <si>
     <t>OPQA-360_1</t>
   </si>
   <si>
-    <t>{"targetType":"posts","targetId":"(OPQA-360_1_id)","content":"Adding Comment on post for Notification Test (ddMMMyyyy_HHmmss)"}</t>
-  </si>
-  <si>
     <t>OPQA-385_1</t>
   </si>
   <si>
     <t>OPQA-385_2</t>
   </si>
   <si>
-    <t>{"targetType":"posts","targetId":"(OPQA-360_1_id)","content":"Adding Comment on post for HPA Notification Test (ddMMMyyyy_HHmmss)"}</t>
-  </si>
-  <si>
-    <t>Verify that user receives a notification if someone commented of his commented post</t>
-  </si>
-  <si>
     <t>OPQA-360_2</t>
   </si>
   <si>
-    <t>status=200||comments.userId=(SYS_USER4)||comments.targetType=Post||comments.targetId=(OPQA-360_2_id)||comments.content=Notification Test</t>
-  </si>
-  <si>
-    <t>{"targetType":"posts","targetId":"(OPQA-360_2_id)","content":"Adding Comment on post for Notification Test (ddMMMyyyy_HHmmss)"}</t>
-  </si>
-  <si>
-    <t>status=200||comments.userId=(SYS_USER4)||comments.targetType=Post||comments.targetId=(OPQA-360_2_id)||comments.content=HPA Notification Test</t>
-  </si>
-  <si>
-    <t>status=200||notify.__typename=authoringTargetComments||notify.issuerProfile.truid=(SYS_USER3)||notify.targetId=(OPQA-360_2_id)</t>
-  </si>
-  <si>
     <t>OPQA-385_3</t>
   </si>
   <si>
@@ -833,6 +788,133 @@
   </si>
   <si>
     <t>OPQA-4143</t>
+  </si>
+  <si>
+    <t>{"title":"Creating Post For HPA Notification API Testing (ddMMMyyyy_HHmmss)","content":"Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing"}</t>
+  </si>
+  <si>
+    <t>OPQA-484</t>
+  </si>
+  <si>
+    <t>Verify that for the given user id, all posts are returned</t>
+  </si>
+  <si>
+    <t>/posts/user/(SYS_USER1)</t>
+  </si>
+  <si>
+    <t>status=200||found=true</t>
+  </si>
+  <si>
+    <t>posts[0].id</t>
+  </si>
+  <si>
+    <t>{"targetType":"posts","targetId":"(OPQA-484_posts[0].id)","content":"Adding Comment on post for Notification Test (ddMMMyyyy_HHmmss)"}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER2)||comments.targetType=Post||comments.targetId=(OPQA-484_posts[0].id)||comments.content=Notification Test</t>
+  </si>
+  <si>
+    <t>{"targetType":"posts","targetId":"(OPQA-484_posts[0].id)","content":"Adding Comment on post for HPA Notification Test (ddMMMyyyy_HHmmss)"}</t>
+  </si>
+  <si>
+    <t>Verify that user receives a notification if someone commented on his commented post</t>
+  </si>
+  <si>
+    <t>1PCONTAINER</t>
+  </si>
+  <si>
+    <t>/container/</t>
+  </si>
+  <si>
+    <t>status=200||type=watchlist||ispublic=true</t>
+  </si>
+  <si>
+    <t>/container/(OPQA-312_id)</t>
+  </si>
+  <si>
+    <t>id||name</t>
+  </si>
+  <si>
+    <t>{
+"name": "(OPQA-312_name)",
+"desc": "Creating public watchList for Notification testing (ddMMMyyyy_HHmmss)",
+"ispublic": "false"
+}</t>
+  </si>
+  <si>
+    <t>{
+"name": "(OPQA-312_name)",
+"desc": "Creating public watchList for Notification testing (ddMMMyyyy_HHmmss)",
+"ispublic": "true"
+}</t>
+  </si>
+  <si>
+    <t>/container/(OPQA-312_id)/items?type=watchlist</t>
+  </si>
+  <si>
+    <t>{
+"items":
+[{
+"id":"(OPQA-360_id)",
+"type":"posts"
+}]
+}</t>
+  </si>
+  <si>
+    <t>{
+"desc": "Creating public watchList for Notification testing (ddMMMyyyy_HHmmss)",
+"name": "Public watchList for Notification testing (ddMMMyyyy_HHmmss)",
+"type":"watchlist",
+"ispublic": true
+}</t>
+  </si>
+  <si>
+    <t>x-1p-user=(SYS_USER3)||Content-Type=application/json</t>
+  </si>
+  <si>
+    <t>{"title":"Creating Post For API Notification Testing TaregetComment (ddMMMyyyy_HHmmss)","content":"Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing Creating Post For API Notification Testing"}</t>
+  </si>
+  <si>
+    <t>{"targetType":"posts","targetId":"(OPQA-360_1_id)","content":"Adding Comment on post for Notification Test Target Comment (ddMMMyyyy_HHmmss)"}</t>
+  </si>
+  <si>
+    <t>id||title</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=AppreciationEvent_V2||notify.issuer=(SYS_USER4)||notify.publicationRef.post.id=(OPQA-360_1_id)||notify.publicationRef.post.title=(OPQA-360_1_title)</t>
+  </si>
+  <si>
+    <t>comments.id||comments.content</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=AppreciationEvent_V2||notify.issuer=(SYS_USER4)||notify.targetType=Comment||notify.publicationRef.comment.content=(OPQA-385_3_comments.content)||notify.publicationRef.comment.post.id=(OPQA-360_1_id)||notify.publicationRef.comment.post.title=(OPQA-360_1_title)</t>
+  </si>
+  <si>
+    <t>{"queryRef":"notifyQrRef_V2","params":{"size":["20"],"byscore":"false"}}</t>
+  </si>
+  <si>
+    <t>status=200||comments.userId=(SYS_USER4)||comments.targetType=Post||comments.targetId=(OPQA-484_posts[0].id)||comments.content=HPA Notification Test</t>
+  </si>
+  <si>
+    <t>status=200||notify.comments.__typename=authoringTargetComments||notify.issuerProfile.truid=(SYS_USER4)||notify.comments.targetId=(OPQA-484_posts[0].id)</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename==PUBLIC_WATCHLIST||notify.issuerProfile.truid=(SYS_USER3)||notify.containerId=(OPQA-312_id)||notify.action=CONTAINER_CREATE</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=PUBLIC_WATCHLIST||notify.issuerProfile.truid=(SYS_USER3)||notify.containerId=(OPQA-312_id)||notify.action=CONTAINER_EDIT_WITH_PERMSSION_CHANGE</t>
+  </si>
+  <si>
+    <t>status=200||notify.__typename=AppreciationEvent_V2||notify.issuer=(SYS_USER3)||notify.publicationRef.comment.targetId=(OPQA-385_comments.id)||notify.publicationRef.post.content=Notification Test (ddMMMyyyy_HHmmss)</t>
+  </si>
+  <si>
+    <t>status=200||notify.cause=WatchedDocumentComment||notify.issuerProfile.truid=(SYS_USER4)||notify.post.id=(OPQA-360_id)||notify.comments.content=(OPQA-385_comments.content)</t>
+  </si>
+  <si>
+    <t>PASS</t>
+  </si>
+  <si>
+    <t>{"queryRef":"notifyQrRef_V2","params":{"size":["20"],"byscore":["true"]}}</t>
   </si>
 </sst>
 </file>
@@ -1249,10 +1331,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L39"/>
+  <dimension ref="A1:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H27" workbookViewId="0">
-      <selection activeCell="M31" sqref="M31"/>
+    <sheetView tabSelected="1" topLeftCell="G34" workbookViewId="0">
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1262,12 +1344,12 @@
     <col min="3" max="3" width="16" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="4" max="4" width="87.85546875" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="47.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="32.140625" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="52.85546875" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="61.85546875" style="5" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="24.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="65.7109375" style="5" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="21.28515625" customWidth="1" collapsed="1"/>
     <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
@@ -1376,7 +1458,7 @@
         <v>35</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="E4" s="1" t="s">
         <v>13</v>
@@ -1406,11 +1488,11 @@
       <c r="E5" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F5" t="s">
+      <c r="F5" s="5" t="s">
         <v>212</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>136</v>
+        <v>275</v>
       </c>
       <c r="I5" t="s">
         <v>33</v>
@@ -1433,7 +1515,7 @@
         <v>35</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>13</v>
@@ -1462,17 +1544,17 @@
       <c r="E7" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F7" s="5" t="s">
         <v>209</v>
       </c>
       <c r="H7" s="5" t="s">
-        <v>136</v>
+        <v>275</v>
       </c>
       <c r="I7" t="s">
         <v>39</v>
       </c>
       <c r="J7" s="5" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="K7" t="s">
         <v>137</v>
@@ -1486,27 +1568,27 @@
         <v>15</v>
       </c>
       <c r="C8" t="s">
-        <v>16</v>
+        <v>250</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>18</v>
+        <v>251</v>
       </c>
       <c r="E8" s="1" t="s">
         <v>13</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G8" s="5"/>
       <c r="H8" s="4" t="s">
-        <v>138</v>
+        <v>259</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="5" t="s">
-        <v>19</v>
+        <v>252</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>17</v>
+        <v>254</v>
       </c>
     </row>
     <row r="9" spans="1:12" ht="45">
@@ -1525,23 +1607,23 @@
       <c r="E9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F9" s="5" t="s">
         <v>212</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>136</v>
+        <v>275</v>
       </c>
       <c r="I9" s="5" t="s">
         <v>92</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>219</v>
+        <v>270</v>
       </c>
       <c r="K9" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="10" spans="1:12" ht="60">
+    <row r="10" spans="1:12" ht="90">
       <c r="A10" s="4" t="s">
         <v>108</v>
       </c>
@@ -1549,20 +1631,20 @@
         <v>110</v>
       </c>
       <c r="C10" t="s">
-        <v>16</v>
+        <v>250</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>102</v>
+        <v>253</v>
       </c>
       <c r="E10" s="1" t="s">
         <v>101</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G10" s="5"/>
       <c r="H10" s="4" t="s">
-        <v>139</v>
+        <v>255</v>
       </c>
       <c r="I10" s="5" t="s">
         <v>92</v>
@@ -1572,7 +1654,7 @@
       </c>
       <c r="K10" s="1"/>
     </row>
-    <row r="11" spans="1:12" ht="60">
+    <row r="11" spans="1:12" ht="90">
       <c r="A11" s="4" t="s">
         <v>109</v>
       </c>
@@ -1580,20 +1662,20 @@
         <v>111</v>
       </c>
       <c r="C11" t="s">
-        <v>16</v>
+        <v>250</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>103</v>
+        <v>253</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>101</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G11" s="5"/>
       <c r="H11" s="4" t="s">
-        <v>140</v>
+        <v>256</v>
       </c>
       <c r="I11" s="5" t="s">
         <v>92</v>
@@ -1619,17 +1701,17 @@
       <c r="E12" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F12" s="5" t="s">
         <v>212</v>
       </c>
       <c r="H12" s="5" t="s">
-        <v>136</v>
+        <v>275</v>
       </c>
       <c r="I12" s="5" t="s">
         <v>92</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>225</v>
+        <v>271</v>
       </c>
       <c r="K12" t="s">
         <v>137</v>
@@ -1652,7 +1734,7 @@
         <v>13</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="9" t="s">
@@ -1660,7 +1742,7 @@
       </c>
       <c r="I13" s="8"/>
       <c r="J13" s="9" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="K13" s="10" t="s">
         <v>46</v>
@@ -1682,17 +1764,17 @@
       <c r="E14" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F14" t="s">
+      <c r="F14" s="5" t="s">
         <v>209</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>136</v>
+        <v>275</v>
       </c>
       <c r="I14" s="8" t="s">
         <v>43</v>
       </c>
       <c r="J14" s="5" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="K14" t="s">
         <v>137</v>
@@ -1715,7 +1797,7 @@
         <v>13</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="11" t="s">
@@ -1746,7 +1828,7 @@
         <v>13</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="11" t="s">
@@ -1776,23 +1858,23 @@
       <c r="E17" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F17" t="s">
+      <c r="F17" s="5" t="s">
         <v>212</v>
       </c>
       <c r="H17" s="5" t="s">
-        <v>136</v>
+        <v>275</v>
       </c>
       <c r="I17" t="s">
         <v>57</v>
       </c>
       <c r="J17" s="5" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="K17" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="75">
+    <row r="18" spans="1:11" ht="105">
       <c r="A18" s="5" t="s">
         <v>100</v>
       </c>
@@ -1800,19 +1882,19 @@
         <v>70</v>
       </c>
       <c r="C18" t="s">
-        <v>16</v>
+        <v>250</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>95</v>
+        <v>257</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F18" t="s">
-        <v>221</v>
+      <c r="F18" s="5" t="s">
+        <v>260</v>
       </c>
       <c r="H18" s="5" t="s">
-        <v>96</v>
+        <v>258</v>
       </c>
       <c r="I18" t="s">
         <v>97</v>
@@ -1838,7 +1920,7 @@
         <v>13</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="9" t="s">
@@ -1848,18 +1930,18 @@
         <v>43</v>
       </c>
       <c r="J19" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="K19" s="10" t="s">
-        <v>29</v>
+        <v>219</v>
+      </c>
+      <c r="K19" s="9" t="s">
+        <v>265</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="45">
-      <c r="A20" s="8" t="s">
-        <v>76</v>
+      <c r="A20" t="s">
+        <v>74</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>134</v>
@@ -1870,17 +1952,17 @@
       <c r="E20" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F20" t="s">
-        <v>220</v>
+      <c r="F20" s="5" t="s">
+        <v>212</v>
       </c>
       <c r="H20" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="I20" s="8" t="s">
-        <v>132</v>
+        <v>275</v>
+      </c>
+      <c r="I20" t="s">
+        <v>72</v>
       </c>
       <c r="J20" s="9" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="K20" t="s">
         <v>137</v>
@@ -1902,28 +1984,28 @@
       <c r="E21" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F21" t="s">
+      <c r="F21" s="5" t="s">
         <v>209</v>
       </c>
       <c r="H21" s="5" t="s">
-        <v>136</v>
+        <v>275</v>
       </c>
       <c r="I21" s="8" t="s">
         <v>72</v>
       </c>
       <c r="J21" s="9" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="K21" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="45">
-      <c r="A22" t="s">
-        <v>74</v>
+      <c r="A22" s="8" t="s">
+        <v>76</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>134</v>
@@ -1934,17 +2016,17 @@
       <c r="E22" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F22" t="s">
-        <v>212</v>
+      <c r="F22" s="5" t="s">
+        <v>217</v>
       </c>
       <c r="H22" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="I22" t="s">
-        <v>72</v>
+        <v>275</v>
+      </c>
+      <c r="I22" s="8" t="s">
+        <v>132</v>
       </c>
       <c r="J22" s="9" t="s">
-        <v>229</v>
+        <v>273</v>
       </c>
       <c r="K22" t="s">
         <v>137</v>
@@ -1967,7 +2049,7 @@
         <v>13</v>
       </c>
       <c r="F23" s="9" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G23" s="8"/>
       <c r="H23" s="9" t="s">
@@ -1998,7 +2080,7 @@
         <v>13</v>
       </c>
       <c r="F24" s="9" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="H24" s="5" t="s">
         <v>50</v>
@@ -2010,7 +2092,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="75">
+    <row r="25" spans="1:11" ht="60">
       <c r="A25" t="s">
         <v>112</v>
       </c>
@@ -2026,429 +2108,456 @@
       <c r="E25" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="F25" t="s">
-        <v>224</v>
+      <c r="F25" s="5" t="s">
+        <v>218</v>
       </c>
       <c r="H25" s="5" t="s">
-        <v>136</v>
+        <v>275</v>
       </c>
       <c r="I25" t="s">
         <v>86</v>
       </c>
       <c r="J25" s="9" t="s">
-        <v>230</v>
+        <v>272</v>
       </c>
       <c r="K25" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="150">
-      <c r="A26" s="8" t="s">
-        <v>232</v>
-      </c>
-      <c r="B26" s="5" t="s">
+    <row r="26" spans="1:11" ht="30">
+      <c r="A26" s="12" t="s">
+        <v>145</v>
+      </c>
+      <c r="B26" s="13" t="s">
+        <v>146</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E26" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F26" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="H26" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="J26" s="5" t="s">
+        <v>149</v>
+      </c>
+      <c r="K26" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" ht="30">
+      <c r="A27" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B27" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D27" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="H27" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="J27" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="K27" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11">
+      <c r="A28" t="s">
+        <v>87</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C28" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="E28" t="s">
+        <v>32</v>
+      </c>
+      <c r="H28"/>
+      <c r="J28" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11">
+      <c r="A29" t="s">
+        <v>90</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="C29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="E29" t="s">
+        <v>32</v>
+      </c>
+      <c r="H29"/>
+      <c r="J29" s="5" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" ht="150">
+      <c r="A30" s="8" t="s">
+        <v>227</v>
+      </c>
+      <c r="B30" s="5" t="s">
         <v>44</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F26" s="9" t="s">
-        <v>213</v>
-      </c>
-      <c r="G26" s="8"/>
-      <c r="H26" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="I26" s="8"/>
-      <c r="J26" s="9" t="s">
-        <v>214</v>
-      </c>
-      <c r="K26" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="27" spans="1:11" ht="45">
-      <c r="A27" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="B27" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C27" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E27" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F27" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="G27" s="8"/>
-      <c r="H27" s="9" t="s">
-        <v>233</v>
-      </c>
-      <c r="I27" t="s">
-        <v>232</v>
-      </c>
-      <c r="J27" s="9" t="s">
-        <v>244</v>
-      </c>
-      <c r="K27" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="28" spans="1:11" ht="30">
-      <c r="A28" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="B28" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D28" s="6" t="s">
-        <v>245</v>
-      </c>
-      <c r="E28" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" s="9" t="s">
-        <v>222</v>
-      </c>
-      <c r="G28" s="8"/>
-      <c r="H28" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="I28" s="8" t="s">
-        <v>243</v>
-      </c>
-      <c r="J28" s="9" t="s">
-        <v>246</v>
-      </c>
-      <c r="K28" s="8"/>
-    </row>
-    <row r="29" spans="1:11" ht="30">
-      <c r="A29" s="8" t="s">
-        <v>253</v>
-      </c>
-      <c r="B29" s="5" t="s">
-        <v>247</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D29" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E29" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F29" t="s">
-        <v>209</v>
-      </c>
-      <c r="H29" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="J29" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K29" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="30" spans="1:11" ht="30">
-      <c r="A30" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" s="16" t="s">
-        <v>249</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D30" s="6" t="s">
-        <v>250</v>
+        <v>45</v>
       </c>
       <c r="E30" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="G30" s="8"/>
-      <c r="H30" s="11" t="s">
-        <v>50</v>
-      </c>
-      <c r="I30" s="8" t="s">
-        <v>232</v>
-      </c>
+      <c r="H30" s="9" t="s">
+        <v>240</v>
+      </c>
+      <c r="I30" s="8"/>
       <c r="J30" s="9" t="s">
-        <v>251</v>
-      </c>
-      <c r="K30" s="8"/>
-    </row>
-    <row r="31" spans="1:11" ht="30">
+        <v>223</v>
+      </c>
+      <c r="K30" s="10" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11">
       <c r="A31" s="8" t="s">
-        <v>254</v>
-      </c>
-      <c r="B31" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="B31" s="16" t="s">
+        <v>242</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="8"/>
+      <c r="I31" s="10"/>
+      <c r="J31" s="9" t="s">
+        <v>244</v>
+      </c>
+      <c r="K31" s="8" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" ht="45">
+      <c r="A32" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="B32" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C32" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F32" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="G32" s="8"/>
+      <c r="H32" s="9" t="s">
+        <v>246</v>
+      </c>
+      <c r="I32" t="s">
+        <v>241</v>
+      </c>
+      <c r="J32" s="9" t="s">
+        <v>247</v>
+      </c>
+      <c r="K32" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" ht="45">
+      <c r="A33" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B33" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="C33" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F33" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="G33" s="8"/>
+      <c r="H33" s="9" t="s">
         <v>248</v>
       </c>
-      <c r="C31" s="1" t="s">
+      <c r="I33" t="s">
+        <v>241</v>
+      </c>
+      <c r="J33" s="9" t="s">
+        <v>268</v>
+      </c>
+      <c r="K33" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" ht="45">
+      <c r="A34" s="8" t="s">
+        <v>237</v>
+      </c>
+      <c r="B34" s="5" t="s">
+        <v>249</v>
+      </c>
+      <c r="C34" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D31" s="6" t="s">
+      <c r="D34" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E31" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F31" t="s">
-        <v>209</v>
-      </c>
-      <c r="H31" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="J31" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="K31" t="s">
+      <c r="E34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F34" t="s">
+        <v>211</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>269</v>
+      </c>
+      <c r="K34" t="s">
         <v>137</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="30">
-      <c r="A32" s="12" t="s">
-        <v>145</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>146</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D32" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F32" t="s">
-        <v>209</v>
-      </c>
-      <c r="H32" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="J32" s="5" t="s">
-        <v>149</v>
-      </c>
-      <c r="K32" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="33" spans="1:11" ht="30">
-      <c r="A33" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>148</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D33" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F33" t="s">
-        <v>209</v>
-      </c>
-      <c r="H33" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="J33" s="5" t="s">
-        <v>150</v>
-      </c>
-      <c r="K33" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="34" spans="1:11">
-      <c r="A34" t="s">
-        <v>87</v>
-      </c>
-      <c r="B34" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C34" t="s">
-        <v>35</v>
-      </c>
-      <c r="D34" s="6" t="s">
-        <v>211</v>
-      </c>
-      <c r="E34" t="s">
-        <v>32</v>
-      </c>
-      <c r="H34"/>
-      <c r="J34" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:11">
-      <c r="A35" t="s">
-        <v>90</v>
+    <row r="35" spans="1:11" ht="150">
+      <c r="A35" s="8" t="s">
+        <v>224</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="C35" t="s">
-        <v>35</v>
+        <v>44</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>27</v>
       </c>
       <c r="D35" s="6" t="s">
-        <v>216</v>
-      </c>
-      <c r="E35" t="s">
-        <v>32</v>
-      </c>
-      <c r="H35"/>
-      <c r="J35" s="5" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:11" ht="150">
+        <v>45</v>
+      </c>
+      <c r="E35" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F35" s="9" t="s">
+        <v>212</v>
+      </c>
+      <c r="G35" s="8"/>
+      <c r="H35" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="I35" s="8"/>
+      <c r="J35" s="9" t="s">
+        <v>213</v>
+      </c>
+      <c r="K35" s="8" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" ht="45">
       <c r="A36" s="8" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D36" s="6" t="s">
-        <v>45</v>
+        <v>28</v>
       </c>
       <c r="E36" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="G36" s="8"/>
       <c r="H36" s="9" t="s">
-        <v>141</v>
-      </c>
-      <c r="I36" s="8"/>
+        <v>262</v>
+      </c>
+      <c r="I36" t="s">
+        <v>224</v>
+      </c>
       <c r="J36" s="9" t="s">
-        <v>231</v>
-      </c>
-      <c r="K36" s="10" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="37" spans="1:11" ht="45">
+        <v>229</v>
+      </c>
+      <c r="K36" s="9" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" ht="30">
       <c r="A37" s="8" t="s">
-        <v>234</v>
+        <v>84</v>
       </c>
       <c r="B37" s="5" t="s">
-        <v>73</v>
+        <v>83</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>27</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>28</v>
+        <v>230</v>
       </c>
       <c r="E37" s="10" t="s">
         <v>13</v>
       </c>
       <c r="F37" s="9" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="G37" s="8"/>
       <c r="H37" s="9" t="s">
-        <v>240</v>
-      </c>
-      <c r="I37" t="s">
+        <v>50</v>
+      </c>
+      <c r="I37" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="J37" s="9" t="s">
+        <v>231</v>
+      </c>
+      <c r="K37" s="8"/>
+    </row>
+    <row r="38" spans="1:11" ht="90">
+      <c r="A38" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="J37" s="9" t="s">
-        <v>239</v>
-      </c>
-      <c r="K37" s="10" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="38" spans="1:11" ht="45">
-      <c r="A38" s="8" t="s">
-        <v>235</v>
-      </c>
       <c r="B38" s="5" t="s">
-        <v>73</v>
-      </c>
-      <c r="C38" s="10" t="s">
-        <v>27</v>
+        <v>232</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>134</v>
       </c>
       <c r="D38" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E38" s="10" t="s">
-        <v>13</v>
-      </c>
-      <c r="F38" s="9" t="s">
-        <v>218</v>
-      </c>
-      <c r="G38" s="8"/>
-      <c r="H38" s="9" t="s">
-        <v>236</v>
-      </c>
-      <c r="I38" t="s">
-        <v>43</v>
-      </c>
-      <c r="J38" s="9" t="s">
-        <v>241</v>
-      </c>
-      <c r="K38" s="10" t="s">
-        <v>29</v>
+        <v>135</v>
+      </c>
+      <c r="E38" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F38" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>266</v>
+      </c>
+      <c r="K38" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="39" spans="1:11" ht="30">
       <c r="A39" s="8" t="s">
-        <v>252</v>
-      </c>
-      <c r="B39" s="5" t="s">
-        <v>237</v>
-      </c>
-      <c r="C39" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" s="16" t="s">
+        <v>234</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" s="6" t="s">
+        <v>235</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="F39" s="9" t="s">
+        <v>218</v>
+      </c>
+      <c r="G39" s="8"/>
+      <c r="H39" s="11" t="s">
+        <v>50</v>
+      </c>
+      <c r="I39" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="J39" s="9" t="s">
+        <v>236</v>
+      </c>
+      <c r="K39" s="8"/>
+    </row>
+    <row r="40" spans="1:11" ht="45">
+      <c r="A40" s="8" t="s">
+        <v>239</v>
+      </c>
+      <c r="B40" s="5" t="s">
+        <v>233</v>
+      </c>
+      <c r="C40" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="D39" s="6" t="s">
+      <c r="D40" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="E39" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F39" t="s">
-        <v>212</v>
-      </c>
-      <c r="H39" s="5" t="s">
-        <v>136</v>
-      </c>
-      <c r="J39" s="5" t="s">
-        <v>242</v>
-      </c>
-      <c r="K39" t="s">
+      <c r="E40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F40" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="H40" s="5" t="s">
+        <v>275</v>
+      </c>
+      <c r="J40" s="5" t="s">
+        <v>264</v>
+      </c>
+      <c r="K40" t="s">
         <v>137</v>
       </c>
     </row>
@@ -5343,14 +5452,94 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F2" sqref="A1:L2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="30" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="30.42578125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="35.7109375" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="22.5703125" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="15.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12">
+      <c r="A1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="45">
+      <c r="A2" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>212</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>267</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="K2" t="s">
+        <v>137</v>
+      </c>
+      <c r="L2" t="s">
+        <v>274</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>